<commit_message>
trying to re factor simulate game
</commit_message>
<xml_diff>
--- a/picks.xlsx
+++ b/picks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdona\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ddb8727edf2838dd/Documents/Development/NCAA_Markov/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06671D6E-1515-43B8-A1C6-82F381F3C2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{06671D6E-1515-43B8-A1C6-82F381F3C2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84996897-F8F3-46CC-90E8-08582306F096}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="288">
   <si>
     <t>started with 119.31</t>
   </si>
@@ -836,6 +836,93 @@
   </si>
   <si>
     <t>UIC</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>indiana md over 135.5</t>
+  </si>
+  <si>
+    <t>Indiana coer +9</t>
+  </si>
+  <si>
+    <t>UNI south illi over 138</t>
+  </si>
+  <si>
+    <t>Southern Ill</t>
+  </si>
+  <si>
+    <t>Illinois St,</t>
+  </si>
+  <si>
+    <t>East car North tex over 122.5</t>
+  </si>
+  <si>
+    <t>east car cover +9</t>
+  </si>
+  <si>
+    <t>North TX</t>
+  </si>
+  <si>
+    <t>KC OR over 142</t>
+  </si>
+  <si>
+    <t>Oral roberts</t>
+  </si>
+  <si>
+    <t>bradley drake over 149</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>murray state cover +14</t>
+  </si>
+  <si>
+    <t>Indiana st</t>
+  </si>
+  <si>
+    <t>ohio st mich over 143.5</t>
+  </si>
+  <si>
+    <t>mich cover +11.5</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>evansville belmont under 154</t>
+  </si>
+  <si>
+    <t>Evansville cover +10.5</t>
+  </si>
+  <si>
+    <t>evansville</t>
+  </si>
+  <si>
+    <t>Memp uab under 158</t>
+  </si>
+  <si>
+    <t>UAB cover +7.5</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Rutgers cover +8.5</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>stanford colo under 155.5</t>
+  </si>
+  <si>
+    <t>Stanford cover +12</t>
+  </si>
+  <si>
+    <t>Colorado</t>
   </si>
 </sst>
 </file>
@@ -1218,17 +1305,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M129"/>
+  <dimension ref="A1:M146"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="7" max="7" width="12" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1298,7 +1385,7 @@
       </c>
       <c r="M3" s="3">
         <f>SUMIF($E:$E,FALSE,$C:$C)/COUNTIF($E:$E,FALSE)</f>
-        <v>0.73540983606557375</v>
+        <v>0.73532258064516121</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1333,7 +1420,7 @@
       </c>
       <c r="M4" s="3">
         <f>SUMIF($E:$E,TRUE,$C:$C)/COUNTIF($E:$E,TRUE)</f>
-        <v>0.72857142857142854</v>
+        <v>0.72859374999999993</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3123,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F126" si="1">IF(E68=TRUE,1,0)</f>
+        <f t="shared" ref="F68:F128" si="1">IF(E68=TRUE,1,0)</f>
         <v>0</v>
       </c>
       <c r="G68" s="3">
@@ -4771,6 +4858,13 @@
       <c r="D127">
         <v>-105</v>
       </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="H127" t="b">
         <v>1</v>
       </c>
@@ -4788,6 +4882,13 @@
       <c r="D128">
         <v>-112</v>
       </c>
+      <c r="E128" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H128" t="b">
         <v>1</v>
       </c>
@@ -4809,8 +4910,261 @@
         <v>1</v>
       </c>
     </row>
+    <row r="130" spans="1:8">
+      <c r="A130" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B130" t="s">
+        <v>260</v>
+      </c>
+      <c r="C130" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D130">
+        <v>-108</v>
+      </c>
+      <c r="H130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B131" t="s">
+        <v>261</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D131">
+        <v>-115</v>
+      </c>
+      <c r="H131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B132" t="s">
+        <v>262</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D132">
+        <v>-102</v>
+      </c>
+      <c r="H132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B133" t="s">
+        <v>265</v>
+      </c>
+      <c r="C133" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D133">
+        <v>-108</v>
+      </c>
+      <c r="H133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B134" t="s">
+        <v>266</v>
+      </c>
+      <c r="C134" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="D134">
+        <v>-112</v>
+      </c>
+      <c r="H134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B135" t="s">
+        <v>268</v>
+      </c>
+      <c r="C135" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D135">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B136" t="s">
+        <v>270</v>
+      </c>
+      <c r="C136" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D136">
+        <v>-112</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B137" t="s">
+        <v>272</v>
+      </c>
+      <c r="C137" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D137">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B138" t="s">
+        <v>274</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D138">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B139" t="s">
+        <v>275</v>
+      </c>
+      <c r="C139" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D139">
+        <v>-108</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B140" t="s">
+        <v>277</v>
+      </c>
+      <c r="C140" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D140">
+        <v>-102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B141" t="s">
+        <v>278</v>
+      </c>
+      <c r="C141" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="D141">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B142" t="s">
+        <v>280</v>
+      </c>
+      <c r="C142" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D142">
+        <v>-102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B143" t="s">
+        <v>281</v>
+      </c>
+      <c r="C143" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="D143">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B144" t="s">
+        <v>283</v>
+      </c>
+      <c r="C144" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D144">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B145" t="s">
+        <v>285</v>
+      </c>
+      <c r="C145" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="D145">
+        <v>-108</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B146" t="s">
+        <v>286</v>
+      </c>
+      <c r="C146" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D146">
+        <v>-110</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H2 E1:F1048576">
+  <conditionalFormatting sqref="E1:F1048576 G2:H2">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4824,21 +5178,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FC2C16-7BDC-417B-A063-6F96F281E8DA}">
-  <dimension ref="A1:R113"/>
+  <dimension ref="A1:R125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView topLeftCell="B105" workbookViewId="0">
+      <selection activeCell="L112" sqref="L112:N112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -4998,7 +5352,7 @@
       </c>
       <c r="R3" s="3">
         <f>SUMIF($E:$E,TRUE,$C:$C)/COUNTIF($E:$E,TRUE)</f>
-        <v>0.63068493150684923</v>
+        <v>0.63202702702702684</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -8214,7 +8568,7 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F111" si="2">IF(E67=TRUE,1,0)</f>
+        <f t="shared" ref="F67:F113" si="2">IF(E67=TRUE,1,0)</f>
         <v>1</v>
       </c>
       <c r="G67" s="3">
@@ -8225,7 +8579,7 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I113" si="3">IF(H67,1,0)*0.5</f>
+        <f t="shared" ref="I67:I115" si="3">IF(H67,1,0)*0.5</f>
         <v>0</v>
       </c>
       <c r="J67">
@@ -10505,15 +10859,45 @@
       <c r="D112">
         <v>-1350</v>
       </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G112" s="3">
+        <f>SUM($F$3:F112)/COUNT($F$3:F112)</f>
+        <v>0.66363636363636369</v>
+      </c>
       <c r="H112" t="b">
         <v>1</v>
       </c>
       <c r="I112">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+        <f>IF(H112,1,0)*1</f>
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+      <c r="K112" s="5" cm="1">
+        <f t="array" ref="K112">IF(E112,_xlfn.IFS(D112="","",I112="","",D112&lt;0,ROUND(I112/D112,3)*-100,D112&gt;0,I112*D112/100),-I112)</f>
+        <v>0.1</v>
+      </c>
+      <c r="L112" s="5">
+        <f>SUM($K$2:K112)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M112" cm="1">
+        <f t="array" ref="M112">IF(E112,_xlfn.IFS(D112="","",J112="","",D112&lt;0,ROUND(J112/D112,3)*-100,D112&gt;0,J112*D112/100),-J112)</f>
+        <v>0.1</v>
+      </c>
+      <c r="N112">
+        <f>SUM($M$2:M112)</f>
+        <v>-1.0799999999999992</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
       <c r="A113" s="2">
         <v>45354</v>
       </c>
@@ -10526,12 +10910,511 @@
       <c r="D113">
         <v>170</v>
       </c>
+      <c r="G113" s="3">
+        <f>SUM($F$3:F113)/COUNT($F$3:F113)</f>
+        <v>0.66363636363636369</v>
+      </c>
       <c r="H113" t="b">
         <v>1</v>
       </c>
       <c r="I113">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
+        <f t="shared" ref="I113:I125" si="4">IF(H113,1,0)*1</f>
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+      <c r="L113" s="5">
+        <f>SUM($K$2:K113)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M113" cm="1">
+        <f t="array" ref="M113">IF(E113,_xlfn.IFS(D113="","",J113="","",D113&lt;0,ROUND(J113/D113,3)*-100,D113&gt;0,J113*D113/100),-J113)</f>
+        <v>-1</v>
+      </c>
+      <c r="N113">
+        <f>SUM($M$2:M113)</f>
+        <v>-2.0799999999999992</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B114" t="s">
+        <v>259</v>
+      </c>
+      <c r="C114" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D114">
+        <v>330</v>
+      </c>
+      <c r="G114" s="3">
+        <f>SUM($F$3:F114)/COUNT($F$3:F114)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H114" t="b">
+        <v>1</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="L114" s="5">
+        <f>SUM($K$2:K114)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M114" cm="1">
+        <f t="array" ref="M114">IF(E114,_xlfn.IFS(D114="","",J114="","",D114&lt;0,ROUND(J114/D114,3)*-100,D114&gt;0,J114*D114/100),-J114)</f>
+        <v>-1</v>
+      </c>
+      <c r="N114">
+        <f>SUM($M$2:M114)</f>
+        <v>-3.0799999999999992</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
+      <c r="A115" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B115" t="s">
+        <v>263</v>
+      </c>
+      <c r="C115" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="D115">
+        <v>-175</v>
+      </c>
+      <c r="G115" s="3">
+        <f>SUM($F$3:F115)/COUNT($F$3:F115)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H115" t="b">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+      <c r="L115" s="5">
+        <f>SUM($K$2:K115)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M115" cm="1">
+        <f t="array" ref="M115">IF(E115,_xlfn.IFS(D115="","",J115="","",D115&lt;0,ROUND(J115/D115,3)*-100,D115&gt;0,J115*D115/100),-J115)</f>
+        <v>-1</v>
+      </c>
+      <c r="N115">
+        <f>SUM($M$2:M115)</f>
+        <v>-4.0799999999999992</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
+      <c r="A116" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B116" t="s">
+        <v>264</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="D116">
+        <v>-230</v>
+      </c>
+      <c r="G116" s="3">
+        <f>SUM($F$3:F116)/COUNT($F$3:F116)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H116" t="b">
+        <v>1</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+      <c r="L116" s="5">
+        <f>SUM($K$2:K116)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M116" cm="1">
+        <f t="array" ref="M116">IF(E116,_xlfn.IFS(D116="","",J116="","",D116&lt;0,ROUND(J116/D116,3)*-100,D116&gt;0,J116*D116/100),-J116)</f>
+        <v>-1</v>
+      </c>
+      <c r="N116">
+        <f>SUM($M$2:M116)</f>
+        <v>-5.0799999999999992</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
+      <c r="A117" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B117" t="s">
+        <v>267</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="D117">
+        <v>-455</v>
+      </c>
+      <c r="G117" s="3">
+        <f>SUM($F$3:F117)/COUNT($F$3:F117)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H117" t="b">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>1</v>
+      </c>
+      <c r="L117" s="5">
+        <f>SUM($K$2:K117)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M117" cm="1">
+        <f t="array" ref="M117">IF(E117,_xlfn.IFS(D117="","",J117="","",D117&lt;0,ROUND(J117/D117,3)*-100,D117&gt;0,J117*D117/100),-J117)</f>
+        <v>-1</v>
+      </c>
+      <c r="N117">
+        <f>SUM($M$2:M117)</f>
+        <v>-6.0799999999999992</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
+      <c r="A118" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B118" t="s">
+        <v>269</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D118">
+        <v>-148</v>
+      </c>
+      <c r="G118" s="3">
+        <f>SUM($F$3:F118)/COUNT($F$3:F118)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H118" t="b">
+        <v>1</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J118">
+        <v>1</v>
+      </c>
+      <c r="L118" s="5">
+        <f>SUM($K$2:K118)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M118" cm="1">
+        <f t="array" ref="M118">IF(E118,_xlfn.IFS(D118="","",J118="","",D118&lt;0,ROUND(J118/D118,3)*-100,D118&gt;0,J118*D118/100),-J118)</f>
+        <v>-1</v>
+      </c>
+      <c r="N118">
+        <f>SUM($M$2:M118)</f>
+        <v>-7.0799999999999992</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
+      <c r="A119" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B119" t="s">
+        <v>271</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D119">
+        <v>-198</v>
+      </c>
+      <c r="G119" s="3">
+        <f>SUM($F$3:F119)/COUNT($F$3:F119)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H119" t="b">
+        <v>1</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <v>1</v>
+      </c>
+      <c r="L119" s="5">
+        <f>SUM($K$2:K119)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M119" cm="1">
+        <f t="array" ref="M119">IF(E119,_xlfn.IFS(D119="","",J119="","",D119&lt;0,ROUND(J119/D119,3)*-100,D119&gt;0,J119*D119/100),-J119)</f>
+        <v>-1</v>
+      </c>
+      <c r="N119">
+        <f>SUM($M$2:M119)</f>
+        <v>-8.0799999999999983</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14">
+      <c r="A120" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B120" t="s">
+        <v>273</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="D120">
+        <v>-1200</v>
+      </c>
+      <c r="G120" s="3">
+        <f>SUM($F$3:F120)/COUNT($F$3:F120)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H120" t="b">
+        <v>1</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J120">
+        <v>1</v>
+      </c>
+      <c r="L120" s="5">
+        <f>SUM($K$2:K120)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M120" cm="1">
+        <f t="array" ref="M120">IF(E120,_xlfn.IFS(D120="","",J120="","",D120&lt;0,ROUND(J120/D120,3)*-100,D120&gt;0,J120*D120/100),-J120)</f>
+        <v>-1</v>
+      </c>
+      <c r="N120">
+        <f>SUM($M$2:M120)</f>
+        <v>-9.0799999999999983</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14">
+      <c r="A121" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B121" t="s">
+        <v>276</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D121">
+        <v>525</v>
+      </c>
+      <c r="G121" s="3">
+        <f>SUM($F$3:F121)/COUNT($F$3:F121)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H121" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J121">
+        <v>1</v>
+      </c>
+      <c r="L121" s="5">
+        <f>SUM($K$2:K121)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M121" cm="1">
+        <f t="array" ref="M121">IF(E121,_xlfn.IFS(D121="","",J121="","",D121&lt;0,ROUND(J121/D121,3)*-100,D121&gt;0,J121*D121/100),-J121)</f>
+        <v>-1</v>
+      </c>
+      <c r="N121">
+        <f>SUM($M$2:M121)</f>
+        <v>-10.079999999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14">
+      <c r="A122" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B122" t="s">
+        <v>279</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D122">
+        <v>470</v>
+      </c>
+      <c r="G122" s="3">
+        <f>SUM($F$3:F122)/COUNT($F$3:F122)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H122" t="b">
+        <v>1</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J122">
+        <v>1</v>
+      </c>
+      <c r="L122" s="5">
+        <f>SUM($K$2:K122)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M122" cm="1">
+        <f t="array" ref="M122">IF(E122,_xlfn.IFS(D122="","",J122="","",D122&lt;0,ROUND(J122/D122,3)*-100,D122&gt;0,J122*D122/100),-J122)</f>
+        <v>-1</v>
+      </c>
+      <c r="N122">
+        <f>SUM($M$2:M122)</f>
+        <v>-11.079999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14">
+      <c r="A123" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B123" t="s">
+        <v>282</v>
+      </c>
+      <c r="C123" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D123">
+        <v>-340</v>
+      </c>
+      <c r="G123" s="3">
+        <f>SUM($F$3:F123)/COUNT($F$3:F123)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H123" t="b">
+        <v>1</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+      <c r="L123" s="5">
+        <f>SUM($K$2:K123)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M123" cm="1">
+        <f t="array" ref="M123">IF(E123,_xlfn.IFS(D123="","",J123="","",D123&lt;0,ROUND(J123/D123,3)*-100,D123&gt;0,J123*D123/100),-J123)</f>
+        <v>-1</v>
+      </c>
+      <c r="N123">
+        <f>SUM($M$2:M123)</f>
+        <v>-12.079999999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14">
+      <c r="A124" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B124" t="s">
+        <v>284</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D124">
+        <v>-410</v>
+      </c>
+      <c r="G124" s="3">
+        <f>SUM($F$3:F124)/COUNT($F$3:F124)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H124" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J124">
+        <v>1</v>
+      </c>
+      <c r="L124" s="5">
+        <f>SUM($K$2:K124)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M124" cm="1">
+        <f t="array" ref="M124">IF(E124,_xlfn.IFS(D124="","",J124="","",D124&lt;0,ROUND(J124/D124,3)*-100,D124&gt;0,J124*D124/100),-J124)</f>
+        <v>-1</v>
+      </c>
+      <c r="N124">
+        <f>SUM($M$2:M124)</f>
+        <v>-13.079999999999998</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14">
+      <c r="A125" s="2">
+        <v>45354</v>
+      </c>
+      <c r="B125" t="s">
+        <v>287</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="D125">
+        <v>-900</v>
+      </c>
+      <c r="G125" s="3">
+        <f>SUM($F$3:F125)/COUNT($F$3:F125)</f>
+        <v>0.66363636363636369</v>
+      </c>
+      <c r="H125" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+      <c r="L125" s="5">
+        <f>SUM($K$2:K125)</f>
+        <v>-1.3800000000000003</v>
+      </c>
+      <c r="M125" cm="1">
+        <f t="array" ref="M125">IF(E125,_xlfn.IFS(D125="","",J125="","",D125&lt;0,ROUND(J125/D125,3)*-100,D125&gt;0,J125*D125/100),-J125)</f>
+        <v>-1</v>
+      </c>
+      <c r="N125">
+        <f>SUM($M$2:M125)</f>
+        <v>-14.079999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to include games on 3/3, set up to calculate team specific time dists
</commit_message>
<xml_diff>
--- a/picks.xlsx
+++ b/picks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ddb8727edf2838dd/Documents/Development/NCAA_Markov/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdona\repos\ncaa_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{06671D6E-1515-43B8-A1C6-82F381F3C2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84996897-F8F3-46CC-90E8-08582306F096}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D637D9F-3CAF-4C29-B679-D55C968C61B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1308,14 +1308,14 @@
   <dimension ref="A1:M146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+      <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="12" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="M3" s="3">
         <f>SUMIF($E:$E,FALSE,$C:$C)/COUNTIF($E:$E,FALSE)</f>
-        <v>0.73532258064516121</v>
+        <v>0.73352112676056336</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="M4" s="3">
         <f>SUMIF($E:$E,TRUE,$C:$C)/COUNTIF($E:$E,TRUE)</f>
-        <v>0.72859374999999993</v>
+        <v>0.73267605633802813</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3210,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F128" si="1">IF(E68=TRUE,1,0)</f>
+        <f t="shared" ref="F68:F138" si="1">IF(E68=TRUE,1,0)</f>
         <v>0</v>
       </c>
       <c r="G68" s="3">
@@ -4865,6 +4865,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="G127" s="3">
+        <f>SUM($F$3:F127)/COUNT($F$3:F127)</f>
+        <v>0.51200000000000001</v>
+      </c>
       <c r="H127" t="b">
         <v>1</v>
       </c>
@@ -4889,6 +4893,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="G128" s="3">
+        <f>SUM($F$3:F128)/COUNT($F$3:F128)</f>
+        <v>0.50793650793650791</v>
+      </c>
       <c r="H128" t="b">
         <v>1</v>
       </c>
@@ -4906,6 +4914,17 @@
       <c r="D129">
         <v>-110</v>
       </c>
+      <c r="E129" t="b">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G129" s="3">
+        <f>SUM($F$3:F129)/COUNT($F$3:F129)</f>
+        <v>0.50393700787401574</v>
+      </c>
       <c r="H129" t="b">
         <v>1</v>
       </c>
@@ -4923,6 +4942,17 @@
       <c r="D130">
         <v>-108</v>
       </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G130" s="3">
+        <f>SUM($F$3:F130)/COUNT($F$3:F130)</f>
+        <v>0.5078125</v>
+      </c>
       <c r="H130" t="b">
         <v>1</v>
       </c>
@@ -4940,6 +4970,17 @@
       <c r="D131">
         <v>-115</v>
       </c>
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G131" s="3">
+        <f>SUM($F$3:F131)/COUNT($F$3:F131)</f>
+        <v>0.51162790697674421</v>
+      </c>
       <c r="H131" t="b">
         <v>1</v>
       </c>
@@ -4957,6 +4998,17 @@
       <c r="D132">
         <v>-102</v>
       </c>
+      <c r="E132" t="b">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G132" s="3">
+        <f>SUM($F$3:F132)/COUNT($F$3:F132)</f>
+        <v>0.51538461538461533</v>
+      </c>
       <c r="H132" t="b">
         <v>1</v>
       </c>
@@ -4974,6 +5026,17 @@
       <c r="D133">
         <v>-108</v>
       </c>
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G133" s="3">
+        <f>SUM($F$3:F133)/COUNT($F$3:F133)</f>
+        <v>0.51908396946564883</v>
+      </c>
       <c r="H133" t="b">
         <v>1</v>
       </c>
@@ -4991,6 +5054,17 @@
       <c r="D134">
         <v>-112</v>
       </c>
+      <c r="E134" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G134" s="3">
+        <f>SUM($F$3:F134)/COUNT($F$3:F134)</f>
+        <v>0.51515151515151514</v>
+      </c>
       <c r="H134" t="b">
         <v>1</v>
       </c>
@@ -5008,6 +5082,20 @@
       <c r="D135">
         <v>-110</v>
       </c>
+      <c r="E135" t="b">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G135" s="3">
+        <f>SUM($F$3:F135)/COUNT($F$3:F135)</f>
+        <v>0.51127819548872178</v>
+      </c>
+      <c r="H135" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" s="2">
@@ -5022,6 +5110,20 @@
       <c r="D136">
         <v>-112</v>
       </c>
+      <c r="E136" t="b">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G136" s="3">
+        <f>SUM($F$3:F136)/COUNT($F$3:F136)</f>
+        <v>0.5074626865671642</v>
+      </c>
+      <c r="H136" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="137" spans="1:8">
       <c r="A137" s="2">
@@ -5036,6 +5138,20 @@
       <c r="D137">
         <v>-110</v>
       </c>
+      <c r="E137" t="b">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G137" s="3">
+        <f>SUM($F$3:F137)/COUNT($F$3:F137)</f>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="H137" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="138" spans="1:8">
       <c r="A138" s="2">
@@ -5050,6 +5166,20 @@
       <c r="D138">
         <v>-115</v>
       </c>
+      <c r="E138" t="b">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G138" s="3">
+        <f>SUM($F$3:F138)/COUNT($F$3:F138)</f>
+        <v>0.51470588235294112</v>
+      </c>
+      <c r="H138" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:8">
       <c r="A139" s="2">
@@ -5064,6 +5194,20 @@
       <c r="D139">
         <v>-108</v>
       </c>
+      <c r="E139" t="b">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <f t="shared" ref="F139:F146" si="2">IF(E139=TRUE,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G139" s="3">
+        <f>SUM($F$3:F139)/COUNT($F$3:F139)</f>
+        <v>0.51094890510948909</v>
+      </c>
+      <c r="H139" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="140" spans="1:8">
       <c r="A140" s="2">
@@ -5078,6 +5222,20 @@
       <c r="D140">
         <v>-102</v>
       </c>
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G140" s="3">
+        <f>SUM($F$3:F140)/COUNT($F$3:F140)</f>
+        <v>0.51449275362318836</v>
+      </c>
+      <c r="H140" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="141" spans="1:8">
       <c r="A141" s="2">
@@ -5092,6 +5250,20 @@
       <c r="D141">
         <v>-110</v>
       </c>
+      <c r="E141" t="b">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G141" s="3">
+        <f>SUM($F$3:F141)/COUNT($F$3:F141)</f>
+        <v>0.51079136690647486</v>
+      </c>
+      <c r="H141" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="142" spans="1:8">
       <c r="A142" s="2">
@@ -5106,6 +5278,20 @@
       <c r="D142">
         <v>-102</v>
       </c>
+      <c r="E142" t="b">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G142" s="3">
+        <f>SUM($F$3:F142)/COUNT($F$3:F142)</f>
+        <v>0.50714285714285712</v>
+      </c>
+      <c r="H142" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" spans="1:8">
       <c r="A143" s="2">
@@ -5120,6 +5306,20 @@
       <c r="D143">
         <v>-110</v>
       </c>
+      <c r="E143" t="b">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G143" s="3">
+        <f>SUM($F$3:F143)/COUNT($F$3:F143)</f>
+        <v>0.50354609929078009</v>
+      </c>
+      <c r="H143" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:8">
       <c r="A144" s="2">
@@ -5134,8 +5334,22 @@
       <c r="D144">
         <v>-105</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144" t="b">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G144" s="3">
+        <f>SUM($F$3:F144)/COUNT($F$3:F144)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
       <c r="A145" s="2">
         <v>45354</v>
       </c>
@@ -5148,8 +5362,19 @@
       <c r="D145">
         <v>-108</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="F145">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G145" s="3">
+        <f>SUM($F$3:F145)/COUNT($F$3:F145)</f>
+        <v>0.49650349650349651</v>
+      </c>
+      <c r="H145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
       <c r="A146" s="2">
         <v>45354</v>
       </c>
@@ -5162,9 +5387,20 @@
       <c r="D146">
         <v>-110</v>
       </c>
+      <c r="F146">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G146" s="3">
+        <f>SUM($F$3:F146)/COUNT($F$3:F146)</f>
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="H146" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:F1048576 G2:H2">
+  <conditionalFormatting sqref="G2:H2 E1:F1048576">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -5180,19 +5416,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FC2C16-7BDC-417B-A063-6F96F281E8DA}">
   <dimension ref="A1:R125"/>
   <sheetViews>
-    <sheetView topLeftCell="B105" workbookViewId="0">
-      <selection activeCell="L112" sqref="L112:N112"/>
+    <sheetView topLeftCell="B99" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113:F125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5294,7 +5530,7 @@
       </c>
       <c r="R2" s="3">
         <f>SUMIF($E:$E,FALSE,$C:$C)/COUNTIF($E:$E,FALSE)</f>
-        <v>0.59048648648648638</v>
+        <v>0.58786046511627899</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -5352,7 +5588,7 @@
       </c>
       <c r="R3" s="3">
         <f>SUMIF($E:$E,TRUE,$C:$C)/COUNTIF($E:$E,TRUE)</f>
-        <v>0.63202702702702684</v>
+        <v>0.63062499999999988</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -8568,7 +8804,7 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F113" si="2">IF(E67=TRUE,1,0)</f>
+        <f t="shared" ref="F67:F125" si="2">IF(E67=TRUE,1,0)</f>
         <v>1</v>
       </c>
       <c r="G67" s="3">
@@ -8579,7 +8815,7 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I115" si="3">IF(H67,1,0)*0.5</f>
+        <f t="shared" ref="I67:I111" si="3">IF(H67,1,0)*0.5</f>
         <v>0</v>
       </c>
       <c r="J67">
@@ -10910,9 +11146,16 @@
       <c r="D113">
         <v>170</v>
       </c>
+      <c r="E113" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G113" s="3">
         <f>SUM($F$3:F113)/COUNT($F$3:F113)</f>
-        <v>0.66363636363636369</v>
+        <v>0.65765765765765771</v>
       </c>
       <c r="H113" t="b">
         <v>1</v>
@@ -10924,9 +11167,13 @@
       <c r="J113">
         <v>1</v>
       </c>
+      <c r="K113" s="5" cm="1">
+        <f t="array" ref="K113">IF(E113,_xlfn.IFS(D113="","",I113="","",D113&lt;0,ROUND(I113/D113,3)*-100,D113&gt;0,I113*D113/100),-I113)</f>
+        <v>-1</v>
+      </c>
       <c r="L113" s="5">
         <f>SUM($K$2:K113)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M113" cm="1">
         <f t="array" ref="M113">IF(E113,_xlfn.IFS(D113="","",J113="","",D113&lt;0,ROUND(J113/D113,3)*-100,D113&gt;0,J113*D113/100),-J113)</f>
@@ -10950,9 +11197,16 @@
       <c r="D114">
         <v>330</v>
       </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G114" s="3">
         <f>SUM($F$3:F114)/COUNT($F$3:F114)</f>
-        <v>0.66363636363636369</v>
+        <v>0.6607142857142857</v>
       </c>
       <c r="H114" t="b">
         <v>1</v>
@@ -10966,15 +11220,15 @@
       </c>
       <c r="L114" s="5">
         <f>SUM($K$2:K114)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M114" cm="1">
         <f t="array" ref="M114">IF(E114,_xlfn.IFS(D114="","",J114="","",D114&lt;0,ROUND(J114/D114,3)*-100,D114&gt;0,J114*D114/100),-J114)</f>
-        <v>-1</v>
+        <v>3.3</v>
       </c>
       <c r="N114">
         <f>SUM($M$2:M114)</f>
-        <v>-3.0799999999999992</v>
+        <v>1.2200000000000006</v>
       </c>
     </row>
     <row r="115" spans="1:14">
@@ -10990,9 +11244,16 @@
       <c r="D115">
         <v>-175</v>
       </c>
+      <c r="E115" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G115" s="3">
         <f>SUM($F$3:F115)/COUNT($F$3:F115)</f>
-        <v>0.66363636363636369</v>
+        <v>0.65486725663716816</v>
       </c>
       <c r="H115" t="b">
         <v>1</v>
@@ -11006,7 +11267,7 @@
       </c>
       <c r="L115" s="5">
         <f>SUM($K$2:K115)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M115" cm="1">
         <f t="array" ref="M115">IF(E115,_xlfn.IFS(D115="","",J115="","",D115&lt;0,ROUND(J115/D115,3)*-100,D115&gt;0,J115*D115/100),-J115)</f>
@@ -11014,7 +11275,7 @@
       </c>
       <c r="N115">
         <f>SUM($M$2:M115)</f>
-        <v>-4.0799999999999992</v>
+        <v>0.22000000000000064</v>
       </c>
     </row>
     <row r="116" spans="1:14">
@@ -11030,9 +11291,16 @@
       <c r="D116">
         <v>-230</v>
       </c>
+      <c r="E116" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G116" s="3">
         <f>SUM($F$3:F116)/COUNT($F$3:F116)</f>
-        <v>0.66363636363636369</v>
+        <v>0.64912280701754388</v>
       </c>
       <c r="H116" t="b">
         <v>1</v>
@@ -11046,7 +11314,7 @@
       </c>
       <c r="L116" s="5">
         <f>SUM($K$2:K116)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M116" cm="1">
         <f t="array" ref="M116">IF(E116,_xlfn.IFS(D116="","",J116="","",D116&lt;0,ROUND(J116/D116,3)*-100,D116&gt;0,J116*D116/100),-J116)</f>
@@ -11054,7 +11322,7 @@
       </c>
       <c r="N116">
         <f>SUM($M$2:M116)</f>
-        <v>-5.0799999999999992</v>
+        <v>-0.77999999999999936</v>
       </c>
     </row>
     <row r="117" spans="1:14">
@@ -11070,9 +11338,16 @@
       <c r="D117">
         <v>-455</v>
       </c>
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G117" s="3">
         <f>SUM($F$3:F117)/COUNT($F$3:F117)</f>
-        <v>0.66363636363636369</v>
+        <v>0.65217391304347827</v>
       </c>
       <c r="H117" t="b">
         <v>1</v>
@@ -11086,15 +11361,15 @@
       </c>
       <c r="L117" s="5">
         <f>SUM($K$2:K117)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M117" cm="1">
         <f t="array" ref="M117">IF(E117,_xlfn.IFS(D117="","",J117="","",D117&lt;0,ROUND(J117/D117,3)*-100,D117&gt;0,J117*D117/100),-J117)</f>
-        <v>-1</v>
+        <v>0.2</v>
       </c>
       <c r="N117">
         <f>SUM($M$2:M117)</f>
-        <v>-6.0799999999999992</v>
+        <v>-0.5799999999999994</v>
       </c>
     </row>
     <row r="118" spans="1:14">
@@ -11110,9 +11385,16 @@
       <c r="D118">
         <v>-148</v>
       </c>
+      <c r="E118" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G118" s="3">
         <f>SUM($F$3:F118)/COUNT($F$3:F118)</f>
-        <v>0.66363636363636369</v>
+        <v>0.64655172413793105</v>
       </c>
       <c r="H118" t="b">
         <v>1</v>
@@ -11126,7 +11408,7 @@
       </c>
       <c r="L118" s="5">
         <f>SUM($K$2:K118)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M118" cm="1">
         <f t="array" ref="M118">IF(E118,_xlfn.IFS(D118="","",J118="","",D118&lt;0,ROUND(J118/D118,3)*-100,D118&gt;0,J118*D118/100),-J118)</f>
@@ -11134,7 +11416,7 @@
       </c>
       <c r="N118">
         <f>SUM($M$2:M118)</f>
-        <v>-7.0799999999999992</v>
+        <v>-1.5799999999999994</v>
       </c>
     </row>
     <row r="119" spans="1:14">
@@ -11150,9 +11432,16 @@
       <c r="D119">
         <v>-198</v>
       </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G119" s="3">
         <f>SUM($F$3:F119)/COUNT($F$3:F119)</f>
-        <v>0.66363636363636369</v>
+        <v>0.6495726495726496</v>
       </c>
       <c r="H119" t="b">
         <v>1</v>
@@ -11166,15 +11455,15 @@
       </c>
       <c r="L119" s="5">
         <f>SUM($K$2:K119)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M119" cm="1">
         <f t="array" ref="M119">IF(E119,_xlfn.IFS(D119="","",J119="","",D119&lt;0,ROUND(J119/D119,3)*-100,D119&gt;0,J119*D119/100),-J119)</f>
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="N119">
         <f>SUM($M$2:M119)</f>
-        <v>-8.0799999999999983</v>
+        <v>-1.0799999999999994</v>
       </c>
     </row>
     <row r="120" spans="1:14">
@@ -11190,9 +11479,16 @@
       <c r="D120">
         <v>-1200</v>
       </c>
+      <c r="E120" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G120" s="3">
         <f>SUM($F$3:F120)/COUNT($F$3:F120)</f>
-        <v>0.66363636363636369</v>
+        <v>0.65254237288135597</v>
       </c>
       <c r="H120" t="b">
         <v>1</v>
@@ -11206,15 +11502,15 @@
       </c>
       <c r="L120" s="5">
         <f>SUM($K$2:K120)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M120" cm="1">
         <f t="array" ref="M120">IF(E120,_xlfn.IFS(D120="","",J120="","",D120&lt;0,ROUND(J120/D120,3)*-100,D120&gt;0,J120*D120/100),-J120)</f>
-        <v>-1</v>
+        <v>0.1</v>
       </c>
       <c r="N120">
         <f>SUM($M$2:M120)</f>
-        <v>-9.0799999999999983</v>
+        <v>-0.97999999999999943</v>
       </c>
     </row>
     <row r="121" spans="1:14">
@@ -11230,9 +11526,16 @@
       <c r="D121">
         <v>525</v>
       </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G121" s="3">
         <f>SUM($F$3:F121)/COUNT($F$3:F121)</f>
-        <v>0.66363636363636369</v>
+        <v>0.6470588235294118</v>
       </c>
       <c r="H121" t="b">
         <v>1</v>
@@ -11246,7 +11549,7 @@
       </c>
       <c r="L121" s="5">
         <f>SUM($K$2:K121)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M121" cm="1">
         <f t="array" ref="M121">IF(E121,_xlfn.IFS(D121="","",J121="","",D121&lt;0,ROUND(J121/D121,3)*-100,D121&gt;0,J121*D121/100),-J121)</f>
@@ -11254,7 +11557,7 @@
       </c>
       <c r="N121">
         <f>SUM($M$2:M121)</f>
-        <v>-10.079999999999998</v>
+        <v>-1.9799999999999995</v>
       </c>
     </row>
     <row r="122" spans="1:14">
@@ -11270,9 +11573,16 @@
       <c r="D122">
         <v>470</v>
       </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G122" s="3">
         <f>SUM($F$3:F122)/COUNT($F$3:F122)</f>
-        <v>0.66363636363636369</v>
+        <v>0.64166666666666672</v>
       </c>
       <c r="H122" t="b">
         <v>1</v>
@@ -11286,7 +11596,7 @@
       </c>
       <c r="L122" s="5">
         <f>SUM($K$2:K122)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M122" cm="1">
         <f t="array" ref="M122">IF(E122,_xlfn.IFS(D122="","",J122="","",D122&lt;0,ROUND(J122/D122,3)*-100,D122&gt;0,J122*D122/100),-J122)</f>
@@ -11294,7 +11604,7 @@
       </c>
       <c r="N122">
         <f>SUM($M$2:M122)</f>
-        <v>-11.079999999999998</v>
+        <v>-2.9799999999999995</v>
       </c>
     </row>
     <row r="123" spans="1:14">
@@ -11310,9 +11620,16 @@
       <c r="D123">
         <v>-340</v>
       </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G123" s="3">
         <f>SUM($F$3:F123)/COUNT($F$3:F123)</f>
-        <v>0.66363636363636369</v>
+        <v>0.64462809917355368</v>
       </c>
       <c r="H123" t="b">
         <v>1</v>
@@ -11326,15 +11643,15 @@
       </c>
       <c r="L123" s="5">
         <f>SUM($K$2:K123)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M123" cm="1">
         <f t="array" ref="M123">IF(E123,_xlfn.IFS(D123="","",J123="","",D123&lt;0,ROUND(J123/D123,3)*-100,D123&gt;0,J123*D123/100),-J123)</f>
-        <v>-1</v>
+        <v>0.3</v>
       </c>
       <c r="N123">
         <f>SUM($M$2:M123)</f>
-        <v>-12.079999999999998</v>
+        <v>-2.6799999999999997</v>
       </c>
     </row>
     <row r="124" spans="1:14">
@@ -11350,9 +11667,16 @@
       <c r="D124">
         <v>-410</v>
       </c>
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G124" s="3">
         <f>SUM($F$3:F124)/COUNT($F$3:F124)</f>
-        <v>0.66363636363636369</v>
+        <v>0.64754098360655743</v>
       </c>
       <c r="H124" t="b">
         <v>1</v>
@@ -11366,15 +11690,15 @@
       </c>
       <c r="L124" s="5">
         <f>SUM($K$2:K124)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M124" cm="1">
         <f t="array" ref="M124">IF(E124,_xlfn.IFS(D124="","",J124="","",D124&lt;0,ROUND(J124/D124,3)*-100,D124&gt;0,J124*D124/100),-J124)</f>
-        <v>-1</v>
+        <v>0.2</v>
       </c>
       <c r="N124">
         <f>SUM($M$2:M124)</f>
-        <v>-13.079999999999998</v>
+        <v>-2.4799999999999995</v>
       </c>
     </row>
     <row r="125" spans="1:14">
@@ -11390,9 +11714,13 @@
       <c r="D125">
         <v>-900</v>
       </c>
+      <c r="F125">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G125" s="3">
         <f>SUM($F$3:F125)/COUNT($F$3:F125)</f>
-        <v>0.66363636363636369</v>
+        <v>0.64227642276422769</v>
       </c>
       <c r="H125" t="b">
         <v>1</v>
@@ -11406,7 +11734,7 @@
       </c>
       <c r="L125" s="5">
         <f>SUM($K$2:K125)</f>
-        <v>-1.3800000000000003</v>
+        <v>-2.3800000000000003</v>
       </c>
       <c r="M125" cm="1">
         <f t="array" ref="M125">IF(E125,_xlfn.IFS(D125="","",J125="","",D125&lt;0,ROUND(J125/D125,3)*-100,D125&gt;0,J125*D125/100),-J125)</f>
@@ -11414,7 +11742,7 @@
       </c>
       <c r="N125">
         <f>SUM($M$2:M125)</f>
-        <v>-14.079999999999998</v>
+        <v>-3.4799999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added team specific time data, have not yet implemented its logic for simulation
</commit_message>
<xml_diff>
--- a/picks.xlsx
+++ b/picks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdona\repos\ncaa_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D637D9F-3CAF-4C29-B679-D55C968C61B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D590D57A-988E-40C5-BF9A-2D294F5C826E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="291">
   <si>
     <t>started with 119.31</t>
   </si>
@@ -923,6 +923,15 @@
   </si>
   <si>
     <t>Colorado</t>
+  </si>
+  <si>
+    <t>Kennesaw st</t>
+  </si>
+  <si>
+    <t>kennes jville under 147.5</t>
+  </si>
+  <si>
+    <t>duke ncstate over 148</t>
   </si>
 </sst>
 </file>
@@ -1305,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M146"/>
+  <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="E145" sqref="E145"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5399,8 +5408,36 @@
         <v>1</v>
       </c>
     </row>
+    <row r="147" spans="1:8">
+      <c r="A147" s="2">
+        <v>45355</v>
+      </c>
+      <c r="B147" t="s">
+        <v>289</v>
+      </c>
+      <c r="C147" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="D147">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" s="2">
+        <v>45355</v>
+      </c>
+      <c r="B148" t="s">
+        <v>290</v>
+      </c>
+      <c r="C148" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="D148">
+        <v>-112</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H2 E1:F1048576">
+  <conditionalFormatting sqref="E1:F1048576 G2:H2">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -5414,10 +5451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FC2C16-7BDC-417B-A063-6F96F281E8DA}">
-  <dimension ref="A1:R125"/>
+  <dimension ref="A1:R127"/>
   <sheetViews>
-    <sheetView topLeftCell="B99" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113:F125"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11745,6 +11782,34 @@
         <v>-3.4799999999999995</v>
       </c>
     </row>
+    <row r="126" spans="1:14">
+      <c r="A126" s="2">
+        <v>45355</v>
+      </c>
+      <c r="B126" t="s">
+        <v>288</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D126">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14">
+      <c r="A127" s="2">
+        <v>45355</v>
+      </c>
+      <c r="B127" t="s">
+        <v>211</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D127">
+        <v>-245</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
started logic for testing NN againts other simulation
</commit_message>
<xml_diff>
--- a/picks.xlsx
+++ b/picks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ddb8727edf2838dd/Documents/Development/NCAA_Markov/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{D590D57A-988E-40C5-BF9A-2D294F5C826E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C2DEACE-B91C-4701-8299-720DB68E891D}"/>
+  <xr:revisionPtr revIDLastSave="491" documentId="13_ncr:1_{D590D57A-988E-40C5-BF9A-2D294F5C826E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D95AAC06-D33B-41A4-9B62-9E94EF328A57}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="390">
   <si>
     <t>started with 119.31</t>
   </si>
@@ -1031,6 +1031,204 @@
   </si>
   <si>
     <t>idaho cover +7</t>
+  </si>
+  <si>
+    <t>ball state</t>
+  </si>
+  <si>
+    <t>kent ball over 142.5</t>
+  </si>
+  <si>
+    <t>liebrty mid tenn over 136</t>
+  </si>
+  <si>
+    <t>liberty cover -5</t>
+  </si>
+  <si>
+    <t>liberty</t>
+  </si>
+  <si>
+    <t>akron</t>
+  </si>
+  <si>
+    <t>eastern mich akron over 131.5</t>
+  </si>
+  <si>
+    <t>eastern mich cover +21</t>
+  </si>
+  <si>
+    <t>vcu duque over 137.5</t>
+  </si>
+  <si>
+    <t>VCU</t>
+  </si>
+  <si>
+    <t>clev st</t>
+  </si>
+  <si>
+    <t>toledo miami oh under 152</t>
+  </si>
+  <si>
+    <t>miami cover +2</t>
+  </si>
+  <si>
+    <t>miami oh</t>
+  </si>
+  <si>
+    <t>bowling green</t>
+  </si>
+  <si>
+    <t>bowling green cover +2</t>
+  </si>
+  <si>
+    <t>loyola md navy over 132.5</t>
+  </si>
+  <si>
+    <t>md cover +6.5</t>
+  </si>
+  <si>
+    <t>harv dart over 137.5</t>
+  </si>
+  <si>
+    <t>harv</t>
+  </si>
+  <si>
+    <t>tulane</t>
+  </si>
+  <si>
+    <t>tulane cover +7</t>
+  </si>
+  <si>
+    <t>vt nh over 140.5</t>
+  </si>
+  <si>
+    <t>vt</t>
+  </si>
+  <si>
+    <t>eastern ky</t>
+  </si>
+  <si>
+    <t>jville cover +8.5</t>
+  </si>
+  <si>
+    <t>queens nc cover +5.5</t>
+  </si>
+  <si>
+    <t>Queens nc stetson under 159.5</t>
+  </si>
+  <si>
+    <t>queens nc</t>
+  </si>
+  <si>
+    <t>purdue ill under 165</t>
+  </si>
+  <si>
+    <t>purdue cover +2.5</t>
+  </si>
+  <si>
+    <t>notre dame cover +16</t>
+  </si>
+  <si>
+    <t>notre dame unc under 139</t>
+  </si>
+  <si>
+    <t>unc</t>
+  </si>
+  <si>
+    <t>va tech</t>
+  </si>
+  <si>
+    <t>providence</t>
+  </si>
+  <si>
+    <t>purdue fw</t>
+  </si>
+  <si>
+    <t>robert morr pfw over 147.5</t>
+  </si>
+  <si>
+    <t>ok cinci under 138</t>
+  </si>
+  <si>
+    <t>cinci cover +5.5</t>
+  </si>
+  <si>
+    <t>oklahoma</t>
+  </si>
+  <si>
+    <t>ok state tx tech over 146</t>
+  </si>
+  <si>
+    <t>det mercy milwaukee under 153</t>
+  </si>
+  <si>
+    <t>milwaukee</t>
+  </si>
+  <si>
+    <t>central mich</t>
+  </si>
+  <si>
+    <t>centram mich NIU over 135</t>
+  </si>
+  <si>
+    <t>north FL cover +4</t>
+  </si>
+  <si>
+    <t>north FL austin peay over 143.5</t>
+  </si>
+  <si>
+    <t>north FL</t>
+  </si>
+  <si>
+    <t>old dominion</t>
+  </si>
+  <si>
+    <t>texas st old dominio over 137</t>
+  </si>
+  <si>
+    <t>old dominio cover +3.5</t>
+  </si>
+  <si>
+    <t>USAFA wy over 137</t>
+  </si>
+  <si>
+    <t>usafa cover +6.5</t>
+  </si>
+  <si>
+    <t>wyoming</t>
+  </si>
+  <si>
+    <t>kansas</t>
+  </si>
+  <si>
+    <t>kansas state cover +12</t>
+  </si>
+  <si>
+    <t>missou cover +12</t>
+  </si>
+  <si>
+    <t>auburn</t>
+  </si>
+  <si>
+    <t>dayton</t>
+  </si>
+  <si>
+    <t>ga tech cover +13.5</t>
+  </si>
+  <si>
+    <t>pittsburgh</t>
+  </si>
+  <si>
+    <t>nv boise st over 141.5</t>
+  </si>
+  <si>
+    <t>nv cover +5.5</t>
+  </si>
+  <si>
+    <t>SDSU UNLV over 135.5</t>
+  </si>
+  <si>
+    <t>SDSU</t>
   </si>
 </sst>
 </file>
@@ -1148,6 +1346,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1413,17 +1615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M168"/>
+  <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="E191" sqref="E191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="7" max="7" width="12" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1493,7 +1695,7 @@
       </c>
       <c r="M3" s="3">
         <f>SUMIF($E:$E,FALSE,$C:$C)/COUNTIF($E:$E,FALSE)</f>
-        <v>0.73352112676056336</v>
+        <v>0.71500000000000019</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1528,7 +1730,7 @@
       </c>
       <c r="M4" s="3">
         <f>SUMIF($E:$E,TRUE,$C:$C)/COUNTIF($E:$E,TRUE)</f>
-        <v>0.73267605633802813</v>
+        <v>0.73136363636363633</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -5470,13 +5672,16 @@
       <c r="D145">
         <v>-108</v>
       </c>
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
       <c r="F145">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G145" s="3">
         <f>SUM($F$3:F145)/COUNT($F$3:F145)</f>
-        <v>0.49650349650349651</v>
+        <v>0.50349650349650354</v>
       </c>
       <c r="H145" t="b">
         <v>1</v>
@@ -5495,13 +5700,16 @@
       <c r="D146">
         <v>-110</v>
       </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
       <c r="F146">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="F146:F149" si="3">IF(E146=TRUE,1,0)</f>
+        <v>1</v>
       </c>
       <c r="G146" s="3">
         <f>SUM($F$3:F146)/COUNT($F$3:F146)</f>
-        <v>0.49305555555555558</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="H146" t="b">
         <v>1</v>
@@ -5520,6 +5728,17 @@
       <c r="D147">
         <v>-110</v>
       </c>
+      <c r="E147" t="b">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G147" s="3">
+        <f>SUM($F$3:F147)/COUNT($F$3:F147)</f>
+        <v>0.50344827586206897</v>
+      </c>
     </row>
     <row r="148" spans="1:8">
       <c r="A148" s="2">
@@ -5534,6 +5753,17 @@
       <c r="D148">
         <v>-112</v>
       </c>
+      <c r="E148" t="b">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G148" s="3">
+        <f>SUM($F$3:F148)/COUNT($F$3:F148)</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="149" spans="1:8">
       <c r="A149" s="2">
@@ -5548,6 +5778,17 @@
       <c r="D149">
         <v>-110</v>
       </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G149" s="3">
+        <f>SUM($F$3:F149)/COUNT($F$3:F149)</f>
+        <v>0.50340136054421769</v>
+      </c>
     </row>
     <row r="150" spans="1:8">
       <c r="A150" s="2">
@@ -5562,6 +5803,17 @@
       <c r="D150">
         <v>-108</v>
       </c>
+      <c r="E150" t="b">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <f t="shared" ref="F150:F207" si="4">IF(E150=TRUE,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G150" s="3">
+        <f>SUM($F$3:F150)/COUNT($F$3:F150)</f>
+        <v>0.5067567567567568</v>
+      </c>
     </row>
     <row r="151" spans="1:8">
       <c r="A151" s="2">
@@ -5576,6 +5828,17 @@
       <c r="D151">
         <v>-108</v>
       </c>
+      <c r="E151" t="b">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G151" s="3">
+        <f>SUM($F$3:F151)/COUNT($F$3:F151)</f>
+        <v>0.50335570469798663</v>
+      </c>
     </row>
     <row r="152" spans="1:8">
       <c r="A152" s="2">
@@ -5590,6 +5853,17 @@
       <c r="D152">
         <v>-115</v>
       </c>
+      <c r="E152" t="b">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G152" s="3">
+        <f>SUM($F$3:F152)/COUNT($F$3:F152)</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="153" spans="1:8">
       <c r="A153" s="2">
@@ -5604,6 +5878,17 @@
       <c r="D153">
         <v>-108</v>
       </c>
+      <c r="E153" t="b">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G153" s="3">
+        <f>SUM($F$3:F153)/COUNT($F$3:F153)</f>
+        <v>0.49668874172185429</v>
+      </c>
     </row>
     <row r="154" spans="1:8">
       <c r="A154" s="2">
@@ -5618,6 +5903,17 @@
       <c r="D154">
         <v>-108</v>
       </c>
+      <c r="E154" t="b">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G154" s="3">
+        <f>SUM($F$3:F154)/COUNT($F$3:F154)</f>
+        <v>0.49342105263157893</v>
+      </c>
     </row>
     <row r="155" spans="1:8">
       <c r="A155" s="2">
@@ -5632,6 +5928,17 @@
       <c r="D155">
         <v>-115</v>
       </c>
+      <c r="E155" t="b">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G155" s="3">
+        <f>SUM($F$3:F155)/COUNT($F$3:F155)</f>
+        <v>0.49019607843137253</v>
+      </c>
     </row>
     <row r="156" spans="1:8">
       <c r="A156" s="2">
@@ -5646,6 +5953,17 @@
       <c r="D156">
         <v>-112</v>
       </c>
+      <c r="E156" t="b">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G156" s="3">
+        <f>SUM($F$3:F156)/COUNT($F$3:F156)</f>
+        <v>0.48701298701298701</v>
+      </c>
     </row>
     <row r="157" spans="1:8">
       <c r="A157" s="2">
@@ -5660,6 +5978,17 @@
       <c r="D157">
         <v>-112</v>
       </c>
+      <c r="E157" t="b">
+        <v>1</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G157" s="3">
+        <f>SUM($F$3:F157)/COUNT($F$3:F157)</f>
+        <v>0.49032258064516127</v>
+      </c>
     </row>
     <row r="158" spans="1:8">
       <c r="A158" s="2">
@@ -5674,6 +6003,17 @@
       <c r="D158">
         <v>-112</v>
       </c>
+      <c r="E158" t="b">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G158" s="3">
+        <f>SUM($F$3:F158)/COUNT($F$3:F158)</f>
+        <v>0.49358974358974361</v>
+      </c>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" s="2">
@@ -5688,6 +6028,17 @@
       <c r="D159">
         <v>-108</v>
       </c>
+      <c r="E159" t="b">
+        <v>1</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G159" s="3">
+        <f>SUM($F$3:F159)/COUNT($F$3:F159)</f>
+        <v>0.49681528662420382</v>
+      </c>
     </row>
     <row r="160" spans="1:8">
       <c r="A160" s="2">
@@ -5702,8 +6053,19 @@
       <c r="D160">
         <v>-110</v>
       </c>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="E160" t="b">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G160" s="3">
+        <f>SUM($F$3:F160)/COUNT($F$3:F160)</f>
+        <v>0.49367088607594939</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
       <c r="A161" s="2">
         <v>45355</v>
       </c>
@@ -5716,8 +6078,19 @@
       <c r="D161">
         <v>-105</v>
       </c>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="E161" t="b">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G161" s="3">
+        <f>SUM($F$3:F161)/COUNT($F$3:F161)</f>
+        <v>0.49056603773584906</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
       <c r="A162" s="2">
         <v>45355</v>
       </c>
@@ -5730,8 +6103,19 @@
       <c r="D162">
         <v>-105</v>
       </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="E162" t="b">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G162" s="3">
+        <f>SUM($F$3:F162)/COUNT($F$3:F162)</f>
+        <v>0.48749999999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
       <c r="A163" s="2">
         <v>45355</v>
       </c>
@@ -5744,8 +6128,19 @@
       <c r="D163">
         <v>-108</v>
       </c>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="E163" t="b">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G163" s="3">
+        <f>SUM($F$3:F163)/COUNT($F$3:F163)</f>
+        <v>0.48447204968944102</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
       <c r="A164" s="2">
         <v>45355</v>
       </c>
@@ -5758,8 +6153,19 @@
       <c r="D164">
         <v>-110</v>
       </c>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="E164" t="b">
+        <v>0</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G164" s="3">
+        <f>SUM($F$3:F164)/COUNT($F$3:F164)</f>
+        <v>0.48148148148148145</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
       <c r="A165" s="2">
         <v>45355</v>
       </c>
@@ -5772,8 +6178,19 @@
       <c r="D165">
         <v>100</v>
       </c>
-    </row>
-    <row r="166" spans="1:4">
+      <c r="E165" t="b">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G165" s="3">
+        <f>SUM($F$3:F165)/COUNT($F$3:F165)</f>
+        <v>0.48466257668711654</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
       <c r="A166" s="2">
         <v>45355</v>
       </c>
@@ -5786,8 +6203,19 @@
       <c r="D166">
         <v>-110</v>
       </c>
-    </row>
-    <row r="167" spans="1:4">
+      <c r="E166" t="b">
+        <v>0</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G166" s="3">
+        <f>SUM($F$3:F166)/COUNT($F$3:F166)</f>
+        <v>0.48170731707317072</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
       <c r="A167" s="2">
         <v>45355</v>
       </c>
@@ -5800,8 +6228,19 @@
       <c r="D167">
         <v>-110</v>
       </c>
-    </row>
-    <row r="168" spans="1:4">
+      <c r="E167" t="b">
+        <v>0</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G167" s="3">
+        <f>SUM($F$3:F167)/COUNT($F$3:F167)</f>
+        <v>0.47878787878787876</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
       <c r="A168" s="2">
         <v>45355</v>
       </c>
@@ -5814,9 +6253,845 @@
       <c r="D168">
         <v>-115</v>
       </c>
+      <c r="E168" t="b">
+        <v>0</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G168" s="3">
+        <f>SUM($F$3:F168)/COUNT($F$3:F168)</f>
+        <v>0.4759036144578313</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B169" t="s">
+        <v>325</v>
+      </c>
+      <c r="C169" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D169">
+        <v>-110</v>
+      </c>
+      <c r="E169" t="b">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G169" s="3">
+        <f>SUM($F$3:F169)/COUNT($F$3:F169)</f>
+        <v>0.47904191616766467</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B170" t="s">
+        <v>326</v>
+      </c>
+      <c r="C170" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="D170">
+        <v>-112</v>
+      </c>
+      <c r="E170" t="b">
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G170" s="3">
+        <f>SUM($F$3:F170)/COUNT($F$3:F170)</f>
+        <v>0.47619047619047616</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B171" t="s">
+        <v>327</v>
+      </c>
+      <c r="C171" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D171">
+        <v>-112</v>
+      </c>
+      <c r="E171" t="b">
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G171" s="3">
+        <f>SUM($F$3:F171)/COUNT($F$3:F171)</f>
+        <v>0.47337278106508873</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B172" t="s">
+        <v>330</v>
+      </c>
+      <c r="C172" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D172">
+        <v>-105</v>
+      </c>
+      <c r="E172" t="b">
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G172" s="3">
+        <f>SUM($F$3:F172)/COUNT($F$3:F172)</f>
+        <v>0.47058823529411764</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B173" t="s">
+        <v>331</v>
+      </c>
+      <c r="C173" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="D173">
+        <v>-108</v>
+      </c>
+      <c r="E173" t="b">
+        <v>1</v>
+      </c>
+      <c r="F173">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G173" s="3">
+        <f>SUM($F$3:F173)/COUNT($F$3:F173)</f>
+        <v>0.47368421052631576</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B174" t="s">
+        <v>332</v>
+      </c>
+      <c r="C174" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="D174">
+        <v>-112</v>
+      </c>
+      <c r="E174" t="b">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G174" s="3">
+        <f>SUM($F$3:F174)/COUNT($F$3:F174)</f>
+        <v>0.47093023255813954</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="B175" t="s">
+        <v>335</v>
+      </c>
+      <c r="C175" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="D175">
+        <v>-110</v>
+      </c>
+      <c r="E175" t="b">
+        <v>0</v>
+      </c>
+      <c r="F175">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G175" s="3">
+        <f>SUM($F$3:F175)/COUNT($F$3:F175)</f>
+        <v>0.46820809248554912</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="B176" t="s">
+        <v>336</v>
+      </c>
+      <c r="C176" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="D176">
+        <v>-108</v>
+      </c>
+      <c r="E176" t="b">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G176" s="3">
+        <f>SUM($F$3:F176)/COUNT($F$3:F176)</f>
+        <v>0.46551724137931033</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7">
+      <c r="B177" t="s">
+        <v>339</v>
+      </c>
+      <c r="C177" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D177">
+        <v>-108</v>
+      </c>
+      <c r="E177" t="b">
+        <v>1</v>
+      </c>
+      <c r="F177">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G177" s="3">
+        <f>SUM($F$3:F177)/COUNT($F$3:F177)</f>
+        <v>0.46857142857142858</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7">
+      <c r="B178" t="s">
+        <v>340</v>
+      </c>
+      <c r="C178" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="D178">
+        <v>-110</v>
+      </c>
+      <c r="E178" t="b">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G178" s="3">
+        <f>SUM($F$3:F178)/COUNT($F$3:F178)</f>
+        <v>0.46590909090909088</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7">
+      <c r="B179" t="s">
+        <v>341</v>
+      </c>
+      <c r="C179" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D179">
+        <v>-110</v>
+      </c>
+      <c r="E179" t="b">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G179" s="3">
+        <f>SUM($F$3:F179)/COUNT($F$3:F179)</f>
+        <v>0.4632768361581921</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7">
+      <c r="B180" t="s">
+        <v>342</v>
+      </c>
+      <c r="C180" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D180">
+        <v>-125</v>
+      </c>
+      <c r="E180" t="b">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G180" s="3">
+        <f>SUM($F$3:F180)/COUNT($F$3:F180)</f>
+        <v>0.46629213483146065</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7">
+      <c r="B181" t="s">
+        <v>345</v>
+      </c>
+      <c r="C181" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="D181">
+        <v>-110</v>
+      </c>
+      <c r="E181" t="b">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G181" s="3">
+        <f>SUM($F$3:F181)/COUNT($F$3:F181)</f>
+        <v>0.46368715083798884</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7">
+      <c r="B182" t="s">
+        <v>346</v>
+      </c>
+      <c r="C182" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="D182">
+        <v>-112</v>
+      </c>
+      <c r="E182" t="b">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G182" s="3">
+        <f>SUM($F$3:F182)/COUNT($F$3:F182)</f>
+        <v>0.46111111111111114</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7">
+      <c r="B183" t="s">
+        <v>349</v>
+      </c>
+      <c r="C183" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D183">
+        <v>-108</v>
+      </c>
+      <c r="E183" t="b">
+        <v>1</v>
+      </c>
+      <c r="F183">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G183" s="3">
+        <f>SUM($F$3:F183)/COUNT($F$3:F183)</f>
+        <v>0.46408839779005523</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7">
+      <c r="B184" t="s">
+        <v>350</v>
+      </c>
+      <c r="C184" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D184">
+        <v>-110</v>
+      </c>
+      <c r="E184" t="b">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G184" s="3">
+        <f>SUM($F$3:F184)/COUNT($F$3:F184)</f>
+        <v>0.46153846153846156</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7">
+      <c r="B185" t="s">
+        <v>351</v>
+      </c>
+      <c r="C185" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D185">
+        <v>-112</v>
+      </c>
+      <c r="E185" t="b">
+        <v>1</v>
+      </c>
+      <c r="F185">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G185" s="3">
+        <f>SUM($F$3:F185)/COUNT($F$3:F185)</f>
+        <v>0.46448087431693991</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7">
+      <c r="B186" t="s">
+        <v>353</v>
+      </c>
+      <c r="C186" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="D186">
+        <v>-115</v>
+      </c>
+      <c r="E186" t="b">
+        <v>1</v>
+      </c>
+      <c r="F186">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G186" s="3">
+        <f>SUM($F$3:F186)/COUNT($F$3:F186)</f>
+        <v>0.46739130434782611</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7">
+      <c r="B187" t="s">
+        <v>354</v>
+      </c>
+      <c r="C187" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="D187">
+        <v>-112</v>
+      </c>
+      <c r="E187" t="b">
+        <v>1</v>
+      </c>
+      <c r="F187">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G187" s="3">
+        <f>SUM($F$3:F187)/COUNT($F$3:F187)</f>
+        <v>0.4702702702702703</v>
+      </c>
+    </row>
+    <row r="188" spans="2:7">
+      <c r="B188" t="s">
+        <v>355</v>
+      </c>
+      <c r="C188" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="D188">
+        <v>-108</v>
+      </c>
+      <c r="E188" t="b">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G188" s="3">
+        <f>SUM($F$3:F188)/COUNT($F$3:F188)</f>
+        <v>0.46774193548387094</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7">
+      <c r="B189" t="s">
+        <v>356</v>
+      </c>
+      <c r="C189" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="D189">
+        <v>-110</v>
+      </c>
+      <c r="E189" t="b">
+        <v>1</v>
+      </c>
+      <c r="F189">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G189" s="3">
+        <f>SUM($F$3:F189)/COUNT($F$3:F189)</f>
+        <v>0.47058823529411764</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7">
+      <c r="B190" t="s">
+        <v>361</v>
+      </c>
+      <c r="C190" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="D190">
+        <v>-105</v>
+      </c>
+      <c r="E190" t="b">
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G190" s="3">
+        <f>SUM($F$3:F190)/COUNT($F$3:F190)</f>
+        <v>0.46808510638297873</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7">
+      <c r="B191" t="s">
+        <v>362</v>
+      </c>
+      <c r="C191" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D191">
+        <v>-108</v>
+      </c>
+      <c r="F191">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G191" s="3">
+        <f>SUM($F$3:F191)/COUNT($F$3:F191)</f>
+        <v>0.46560846560846558</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7">
+      <c r="B192" t="s">
+        <v>363</v>
+      </c>
+      <c r="C192" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D192">
+        <v>-110</v>
+      </c>
+      <c r="F192">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G192" s="3">
+        <f>SUM($F$3:F192)/COUNT($F$3:F192)</f>
+        <v>0.4631578947368421</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7">
+      <c r="B193" t="s">
+        <v>365</v>
+      </c>
+      <c r="C193" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D193">
+        <v>-105</v>
+      </c>
+      <c r="F193">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G193" s="3">
+        <f>SUM($F$3:F193)/COUNT($F$3:F193)</f>
+        <v>0.4607329842931937</v>
+      </c>
+    </row>
+    <row r="194" spans="2:7">
+      <c r="B194" t="s">
+        <v>366</v>
+      </c>
+      <c r="C194" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="D194">
+        <v>-105</v>
+      </c>
+      <c r="F194">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G194" s="3">
+        <f>SUM($F$3:F194)/COUNT($F$3:F194)</f>
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7">
+      <c r="B195" t="s">
+        <v>369</v>
+      </c>
+      <c r="C195" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D195">
+        <v>-115</v>
+      </c>
+      <c r="F195">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G195" s="3">
+        <f>SUM($F$3:F195)/COUNT($F$3:F195)</f>
+        <v>0.45595854922279794</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7">
+      <c r="B196" t="s">
+        <v>370</v>
+      </c>
+      <c r="C196" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D196">
+        <v>-112</v>
+      </c>
+      <c r="F196">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G196" s="3">
+        <f>SUM($F$3:F196)/COUNT($F$3:F196)</f>
+        <v>0.45360824742268041</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7">
+      <c r="B197" t="s">
+        <v>371</v>
+      </c>
+      <c r="C197" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="D197">
+        <v>-112</v>
+      </c>
+      <c r="F197">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G197" s="3">
+        <f>SUM($F$3:F197)/COUNT($F$3:F197)</f>
+        <v>0.45128205128205129</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7">
+      <c r="B198" t="s">
+        <v>374</v>
+      </c>
+      <c r="C198" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="D198">
+        <v>100</v>
+      </c>
+      <c r="F198">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G198" s="3">
+        <f>SUM($F$3:F198)/COUNT($F$3:F198)</f>
+        <v>0.44897959183673469</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7">
+      <c r="B199" t="s">
+        <v>375</v>
+      </c>
+      <c r="C199" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="D199">
+        <v>-105</v>
+      </c>
+      <c r="F199">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G199" s="3">
+        <f>SUM($F$3:F199)/COUNT($F$3:F199)</f>
+        <v>0.4467005076142132</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7">
+      <c r="B200" t="s">
+        <v>376</v>
+      </c>
+      <c r="C200" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D200">
+        <v>-102</v>
+      </c>
+      <c r="F200">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G200" s="3">
+        <f>SUM($F$3:F200)/COUNT($F$3:F200)</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="201" spans="2:7">
+      <c r="B201" t="s">
+        <v>377</v>
+      </c>
+      <c r="C201" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D201">
+        <v>-105</v>
+      </c>
+      <c r="F201">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G201" s="3">
+        <f>SUM($F$3:F201)/COUNT($F$3:F201)</f>
+        <v>0.44221105527638194</v>
+      </c>
+    </row>
+    <row r="202" spans="2:7">
+      <c r="B202" t="s">
+        <v>380</v>
+      </c>
+      <c r="C202" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D202">
+        <v>-105</v>
+      </c>
+      <c r="F202">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G202" s="3">
+        <f>SUM($F$3:F202)/COUNT($F$3:F202)</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="203" spans="2:7">
+      <c r="B203" t="s">
+        <v>381</v>
+      </c>
+      <c r="C203" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D203">
+        <v>-122</v>
+      </c>
+      <c r="F203">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G203" s="3">
+        <f>SUM($F$3:F203)/COUNT($F$3:F203)</f>
+        <v>0.43781094527363185</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7">
+      <c r="B204" t="s">
+        <v>384</v>
+      </c>
+      <c r="C204" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D204">
+        <v>-105</v>
+      </c>
+      <c r="F204">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G204" s="3">
+        <f>SUM($F$3:F204)/COUNT($F$3:F204)</f>
+        <v>0.43564356435643564</v>
+      </c>
+    </row>
+    <row r="205" spans="2:7">
+      <c r="B205" t="s">
+        <v>386</v>
+      </c>
+      <c r="C205" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D205">
+        <v>-110</v>
+      </c>
+      <c r="F205">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G205" s="3">
+        <f>SUM($F$3:F205)/COUNT($F$3:F205)</f>
+        <v>0.43349753694581283</v>
+      </c>
+    </row>
+    <row r="206" spans="2:7">
+      <c r="B206" t="s">
+        <v>387</v>
+      </c>
+      <c r="C206" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D206">
+        <v>-105</v>
+      </c>
+      <c r="F206">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G206" s="3">
+        <f>SUM($F$3:F206)/COUNT($F$3:F206)</f>
+        <v>0.43137254901960786</v>
+      </c>
+    </row>
+    <row r="207" spans="2:7">
+      <c r="B207" t="s">
+        <v>388</v>
+      </c>
+      <c r="C207" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="D207">
+        <v>-110</v>
+      </c>
+      <c r="F207">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G207" s="3">
+        <f>SUM($F$3:F207)/COUNT($F$3:F207)</f>
+        <v>0.42926829268292682</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:F1048576 G2:H2">
+  <conditionalFormatting sqref="G2:H2 E1:F1048576">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -5830,10 +7105,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FC2C16-7BDC-417B-A063-6F96F281E8DA}">
-  <dimension ref="A1:R146"/>
+  <dimension ref="A1:R180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5946,7 +7221,7 @@
       </c>
       <c r="R2" s="3">
         <f>SUMIF($E:$E,FALSE,$C:$C)/COUNTIF($E:$E,FALSE)</f>
-        <v>0.58786046511627899</v>
+        <v>0.59698245614035084</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -6004,7 +7279,7 @@
       </c>
       <c r="R3" s="3">
         <f>SUMIF($E:$E,TRUE,$C:$C)/COUNTIF($E:$E,TRUE)</f>
-        <v>0.63062499999999988</v>
+        <v>0.6327102803738317</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -12130,13 +13405,16 @@
       <c r="D125">
         <v>-900</v>
       </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
       <c r="F125">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125" s="3">
         <f>SUM($F$3:F125)/COUNT($F$3:F125)</f>
-        <v>0.64227642276422769</v>
+        <v>0.65040650406504064</v>
       </c>
       <c r="H125" t="b">
         <v>1</v>
@@ -12154,11 +13432,11 @@
       </c>
       <c r="M125" cm="1">
         <f t="array" ref="M125">IF(E125,_xlfn.IFS(D125="","",J125="","",D125&lt;0,ROUND(J125/D125,3)*-100,D125&gt;0,J125*D125/100),-J125)</f>
-        <v>-1</v>
+        <v>0.1</v>
       </c>
       <c r="N125">
         <f>SUM($M$2:M125)</f>
-        <v>-3.4799999999999995</v>
+        <v>-2.3799999999999994</v>
       </c>
     </row>
     <row r="126" spans="1:14">
@@ -12174,6 +13452,39 @@
       <c r="D126">
         <v>-180</v>
       </c>
+      <c r="E126" t="b">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <f t="shared" ref="F126:F180" si="5">IF(E126=TRUE,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G126" s="3">
+        <f>SUM($F$3:F126)/COUNT($F$3:F126)</f>
+        <v>0.64516129032258063</v>
+      </c>
+      <c r="H126" t="b">
+        <v>1</v>
+      </c>
+      <c r="I126">
+        <f t="shared" ref="I126:I180" si="6">IF(H126,1,0)*1</f>
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <v>2</v>
+      </c>
+      <c r="L126" s="5">
+        <f>SUM($K$2:K126)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M126" cm="1">
+        <f t="array" ref="M126">IF(E126,_xlfn.IFS(D126="","",J126="","",D126&lt;0,ROUND(J126/D126,3)*-100,D126&gt;0,J126*D126/100),-J126)</f>
+        <v>-2</v>
+      </c>
+      <c r="N126">
+        <f>SUM($M$2:M126)</f>
+        <v>-4.379999999999999</v>
+      </c>
     </row>
     <row r="127" spans="1:14">
       <c r="A127" s="2">
@@ -12188,6 +13499,39 @@
       <c r="D127">
         <v>-245</v>
       </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G127" s="3">
+        <f>SUM($F$3:F127)/COUNT($F$3:F127)</f>
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="H127" t="b">
+        <v>1</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J127">
+        <v>3</v>
+      </c>
+      <c r="L127" s="5">
+        <f>SUM($K$2:K127)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M127" cm="1">
+        <f t="array" ref="M127">IF(E127,_xlfn.IFS(D127="","",J127="","",D127&lt;0,ROUND(J127/D127,3)*-100,D127&gt;0,J127*D127/100),-J127)</f>
+        <v>1.2</v>
+      </c>
+      <c r="N127">
+        <f>SUM($M$2:M127)</f>
+        <v>-3.1799999999999988</v>
+      </c>
     </row>
     <row r="128" spans="1:14">
       <c r="A128" s="2">
@@ -12202,8 +13546,41 @@
       <c r="D128">
         <v>142</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G128" s="3">
+        <f>SUM($F$3:F128)/COUNT($F$3:F128)</f>
+        <v>0.65079365079365081</v>
+      </c>
+      <c r="H128" t="b">
+        <v>1</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <v>4</v>
+      </c>
+      <c r="L128" s="5">
+        <f>SUM($K$2:K128)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M128" cm="1">
+        <f t="array" ref="M128">IF(E128,_xlfn.IFS(D128="","",J128="","",D128&lt;0,ROUND(J128/D128,3)*-100,D128&gt;0,J128*D128/100),-J128)</f>
+        <v>5.68</v>
+      </c>
+      <c r="N128">
+        <f>SUM($M$2:M128)</f>
+        <v>2.5000000000000009</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14">
       <c r="A129" s="2">
         <v>45355</v>
       </c>
@@ -12216,8 +13593,41 @@
       <c r="D129">
         <v>-1050</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G129" s="3">
+        <f>SUM($F$3:F129)/COUNT($F$3:F129)</f>
+        <v>0.65354330708661412</v>
+      </c>
+      <c r="H129" t="b">
+        <v>1</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J129">
+        <v>5</v>
+      </c>
+      <c r="L129" s="5">
+        <f>SUM($K$2:K129)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M129" cm="1">
+        <f t="array" ref="M129">IF(E129,_xlfn.IFS(D129="","",J129="","",D129&lt;0,ROUND(J129/D129,3)*-100,D129&gt;0,J129*D129/100),-J129)</f>
+        <v>0.5</v>
+      </c>
+      <c r="N129">
+        <f>SUM($M$2:M129)</f>
+        <v>3.0000000000000009</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14">
       <c r="A130" s="2">
         <v>45355</v>
       </c>
@@ -12230,8 +13640,41 @@
       <c r="D130">
         <v>180</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130" t="b">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G130" s="3">
+        <f>SUM($F$3:F130)/COUNT($F$3:F130)</f>
+        <v>0.6484375</v>
+      </c>
+      <c r="H130" t="b">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J130">
+        <v>6</v>
+      </c>
+      <c r="L130" s="5">
+        <f>SUM($K$2:K130)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M130" cm="1">
+        <f t="array" ref="M130">IF(E130,_xlfn.IFS(D130="","",J130="","",D130&lt;0,ROUND(J130/D130,3)*-100,D130&gt;0,J130*D130/100),-J130)</f>
+        <v>-6</v>
+      </c>
+      <c r="N130">
+        <f>SUM($M$2:M130)</f>
+        <v>-2.9999999999999991</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14">
       <c r="A131" s="2">
         <v>45355</v>
       </c>
@@ -12244,8 +13687,41 @@
       <c r="D131">
         <v>-130</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G131" s="3">
+        <f>SUM($F$3:F131)/COUNT($F$3:F131)</f>
+        <v>0.65116279069767447</v>
+      </c>
+      <c r="H131" t="b">
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J131">
+        <v>7</v>
+      </c>
+      <c r="L131" s="5">
+        <f>SUM($K$2:K131)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M131" cm="1">
+        <f t="array" ref="M131">IF(E131,_xlfn.IFS(D131="","",J131="","",D131&lt;0,ROUND(J131/D131,3)*-100,D131&gt;0,J131*D131/100),-J131)</f>
+        <v>5.4</v>
+      </c>
+      <c r="N131">
+        <f>SUM($M$2:M131)</f>
+        <v>2.4000000000000012</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14">
       <c r="A132" s="2">
         <v>45355</v>
       </c>
@@ -12258,8 +13734,41 @@
       <c r="D132">
         <v>-175</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132" t="b">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G132" s="3">
+        <f>SUM($F$3:F132)/COUNT($F$3:F132)</f>
+        <v>0.65384615384615385</v>
+      </c>
+      <c r="H132" t="b">
+        <v>1</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J132">
+        <v>8</v>
+      </c>
+      <c r="L132" s="5">
+        <f>SUM($K$2:K132)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M132" cm="1">
+        <f t="array" ref="M132">IF(E132,_xlfn.IFS(D132="","",J132="","",D132&lt;0,ROUND(J132/D132,3)*-100,D132&gt;0,J132*D132/100),-J132)</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N132">
+        <f>SUM($M$2:M132)</f>
+        <v>7.0000000000000009</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14">
       <c r="A133" s="2">
         <v>45355</v>
       </c>
@@ -12272,8 +13781,41 @@
       <c r="D133">
         <v>-395</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G133" s="3">
+        <f>SUM($F$3:F133)/COUNT($F$3:F133)</f>
+        <v>0.65648854961832059</v>
+      </c>
+      <c r="H133" t="b">
+        <v>1</v>
+      </c>
+      <c r="I133">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>9</v>
+      </c>
+      <c r="L133" s="5">
+        <f>SUM($K$2:K133)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M133" cm="1">
+        <f t="array" ref="M133">IF(E133,_xlfn.IFS(D133="","",J133="","",D133&lt;0,ROUND(J133/D133,3)*-100,D133&gt;0,J133*D133/100),-J133)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N133">
+        <f>SUM($M$2:M133)</f>
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14">
       <c r="A134" s="2">
         <v>45355</v>
       </c>
@@ -12286,8 +13828,41 @@
       <c r="D134">
         <v>-440</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G134" s="3">
+        <f>SUM($F$3:F134)/COUNT($F$3:F134)</f>
+        <v>0.65151515151515149</v>
+      </c>
+      <c r="H134" t="b">
+        <v>1</v>
+      </c>
+      <c r="I134">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <v>10</v>
+      </c>
+      <c r="L134" s="5">
+        <f>SUM($K$2:K134)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M134" cm="1">
+        <f t="array" ref="M134">IF(E134,_xlfn.IFS(D134="","",J134="","",D134&lt;0,ROUND(J134/D134,3)*-100,D134&gt;0,J134*D134/100),-J134)</f>
+        <v>-10</v>
+      </c>
+      <c r="N134">
+        <f>SUM($M$2:M134)</f>
+        <v>-0.69999999999999929</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14">
       <c r="A135" s="2">
         <v>45355</v>
       </c>
@@ -12300,8 +13875,41 @@
       <c r="D135">
         <v>-180</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G135" s="3">
+        <f>SUM($F$3:F135)/COUNT($F$3:F135)</f>
+        <v>0.65413533834586468</v>
+      </c>
+      <c r="H135" t="b">
+        <v>1</v>
+      </c>
+      <c r="I135">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J135">
+        <v>11</v>
+      </c>
+      <c r="L135" s="5">
+        <f>SUM($K$2:K135)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M135" cm="1">
+        <f t="array" ref="M135">IF(E135,_xlfn.IFS(D135="","",J135="","",D135&lt;0,ROUND(J135/D135,3)*-100,D135&gt;0,J135*D135/100),-J135)</f>
+        <v>6.1</v>
+      </c>
+      <c r="N135">
+        <f>SUM($M$2:M135)</f>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14">
       <c r="A136" s="2">
         <v>45355</v>
       </c>
@@ -12314,8 +13922,41 @@
       <c r="D136">
         <v>-185</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136" t="b">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G136" s="3">
+        <f>SUM($F$3:F136)/COUNT($F$3:F136)</f>
+        <v>0.65671641791044777</v>
+      </c>
+      <c r="H136" t="b">
+        <v>1</v>
+      </c>
+      <c r="I136">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>12</v>
+      </c>
+      <c r="L136" s="5">
+        <f>SUM($K$2:K136)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M136" cm="1">
+        <f t="array" ref="M136">IF(E136,_xlfn.IFS(D136="","",J136="","",D136&lt;0,ROUND(J136/D136,3)*-100,D136&gt;0,J136*D136/100),-J136)</f>
+        <v>6.5</v>
+      </c>
+      <c r="N136">
+        <f>SUM($M$2:M136)</f>
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14">
       <c r="A137" s="2">
         <v>45355</v>
       </c>
@@ -12328,8 +13969,41 @@
       <c r="D137">
         <v>-1200</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137" t="b">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G137" s="3">
+        <f>SUM($F$3:F137)/COUNT($F$3:F137)</f>
+        <v>0.65925925925925921</v>
+      </c>
+      <c r="H137" t="b">
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <v>13</v>
+      </c>
+      <c r="L137" s="5">
+        <f>SUM($K$2:K137)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M137" cm="1">
+        <f t="array" ref="M137">IF(E137,_xlfn.IFS(D137="","",J137="","",D137&lt;0,ROUND(J137/D137,3)*-100,D137&gt;0,J137*D137/100),-J137)</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="N137">
+        <f>SUM($M$2:M137)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14">
       <c r="A138" s="2">
         <v>45355</v>
       </c>
@@ -12342,8 +14016,41 @@
       <c r="D138">
         <v>185</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138" t="b">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G138" s="3">
+        <f>SUM($F$3:F138)/COUNT($F$3:F138)</f>
+        <v>0.65441176470588236</v>
+      </c>
+      <c r="H138" t="b">
+        <v>1</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J138">
+        <v>14</v>
+      </c>
+      <c r="L138" s="5">
+        <f>SUM($K$2:K138)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M138" cm="1">
+        <f t="array" ref="M138">IF(E138,_xlfn.IFS(D138="","",J138="","",D138&lt;0,ROUND(J138/D138,3)*-100,D138&gt;0,J138*D138/100),-J138)</f>
+        <v>-14</v>
+      </c>
+      <c r="N138">
+        <f>SUM($M$2:M138)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14">
       <c r="A139" s="2">
         <v>45355</v>
       </c>
@@ -12356,8 +14063,41 @@
       <c r="D139">
         <v>-142</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G139" s="3">
+        <f>SUM($F$3:F139)/COUNT($F$3:F139)</f>
+        <v>0.65693430656934304</v>
+      </c>
+      <c r="H139" t="b">
+        <v>1</v>
+      </c>
+      <c r="I139">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J139">
+        <v>15</v>
+      </c>
+      <c r="L139" s="5">
+        <f>SUM($K$2:K139)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M139" cm="1">
+        <f t="array" ref="M139">IF(E139,_xlfn.IFS(D139="","",J139="","",D139&lt;0,ROUND(J139/D139,3)*-100,D139&gt;0,J139*D139/100),-J139)</f>
+        <v>10.6</v>
+      </c>
+      <c r="N139">
+        <f>SUM($M$2:M139)</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14">
       <c r="A140" s="2">
         <v>45355</v>
       </c>
@@ -12370,8 +14110,41 @@
       <c r="D140">
         <v>-192</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140" t="b">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G140" s="3">
+        <f>SUM($F$3:F140)/COUNT($F$3:F140)</f>
+        <v>0.65217391304347827</v>
+      </c>
+      <c r="H140" t="b">
+        <v>1</v>
+      </c>
+      <c r="I140">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J140">
+        <v>16</v>
+      </c>
+      <c r="L140" s="5">
+        <f>SUM($K$2:K140)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M140" cm="1">
+        <f t="array" ref="M140">IF(E140,_xlfn.IFS(D140="","",J140="","",D140&lt;0,ROUND(J140/D140,3)*-100,D140&gt;0,J140*D140/100),-J140)</f>
+        <v>-16</v>
+      </c>
+      <c r="N140">
+        <f>SUM($M$2:M140)</f>
+        <v>-6.4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14">
       <c r="A141" s="2">
         <v>45355</v>
       </c>
@@ -12384,8 +14157,41 @@
       <c r="D141">
         <v>-375</v>
       </c>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G141" s="3">
+        <f>SUM($F$3:F141)/COUNT($F$3:F141)</f>
+        <v>0.65467625899280579</v>
+      </c>
+      <c r="H141" t="b">
+        <v>1</v>
+      </c>
+      <c r="I141">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J141">
+        <v>17</v>
+      </c>
+      <c r="L141" s="5">
+        <f>SUM($K$2:K141)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M141" cm="1">
+        <f t="array" ref="M141">IF(E141,_xlfn.IFS(D141="","",J141="","",D141&lt;0,ROUND(J141/D141,3)*-100,D141&gt;0,J141*D141/100),-J141)</f>
+        <v>4.5</v>
+      </c>
+      <c r="N141">
+        <f>SUM($M$2:M141)</f>
+        <v>-1.9000000000000004</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14">
       <c r="A142" s="2">
         <v>45355</v>
       </c>
@@ -12398,8 +14204,41 @@
       <c r="D142">
         <v>-395</v>
       </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G142" s="3">
+        <f>SUM($F$3:F142)/COUNT($F$3:F142)</f>
+        <v>0.65714285714285714</v>
+      </c>
+      <c r="H142" t="b">
+        <v>1</v>
+      </c>
+      <c r="I142">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>18</v>
+      </c>
+      <c r="L142" s="5">
+        <f>SUM($K$2:K142)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M142" cm="1">
+        <f t="array" ref="M142">IF(E142,_xlfn.IFS(D142="","",J142="","",D142&lt;0,ROUND(J142/D142,3)*-100,D142&gt;0,J142*D142/100),-J142)</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N142">
+        <f>SUM($M$2:M142)</f>
+        <v>2.6999999999999993</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14">
       <c r="A143" s="2">
         <v>45355</v>
       </c>
@@ -12412,8 +14251,41 @@
       <c r="D143">
         <v>-575</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="E143" t="b">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G143" s="3">
+        <f>SUM($F$3:F143)/COUNT($F$3:F143)</f>
+        <v>0.65957446808510634</v>
+      </c>
+      <c r="H143" t="b">
+        <v>1</v>
+      </c>
+      <c r="I143">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>19</v>
+      </c>
+      <c r="L143" s="5">
+        <f>SUM($K$2:K143)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M143" cm="1">
+        <f t="array" ref="M143">IF(E143,_xlfn.IFS(D143="","",J143="","",D143&lt;0,ROUND(J143/D143,3)*-100,D143&gt;0,J143*D143/100),-J143)</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="N143">
+        <f>SUM($M$2:M143)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14">
       <c r="A144" s="2">
         <v>45355</v>
       </c>
@@ -12426,8 +14298,41 @@
       <c r="D144">
         <v>-205</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144" t="b">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G144" s="3">
+        <f>SUM($F$3:F144)/COUNT($F$3:F144)</f>
+        <v>0.65492957746478875</v>
+      </c>
+      <c r="H144" t="b">
+        <v>1</v>
+      </c>
+      <c r="I144">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>20</v>
+      </c>
+      <c r="L144" s="5">
+        <f>SUM($K$2:K144)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M144" cm="1">
+        <f t="array" ref="M144">IF(E144,_xlfn.IFS(D144="","",J144="","",D144&lt;0,ROUND(J144/D144,3)*-100,D144&gt;0,J144*D144/100),-J144)</f>
+        <v>-20</v>
+      </c>
+      <c r="N144">
+        <f>SUM($M$2:M144)</f>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
       <c r="A145" s="2">
         <v>45355</v>
       </c>
@@ -12440,8 +14345,41 @@
       <c r="D145">
         <v>-440</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G145" s="3">
+        <f>SUM($F$3:F145)/COUNT($F$3:F145)</f>
+        <v>0.65734265734265729</v>
+      </c>
+      <c r="H145" t="b">
+        <v>1</v>
+      </c>
+      <c r="I145">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J145">
+        <v>21</v>
+      </c>
+      <c r="L145" s="5">
+        <f>SUM($K$2:K145)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M145" cm="1">
+        <f t="array" ref="M145">IF(E145,_xlfn.IFS(D145="","",J145="","",D145&lt;0,ROUND(J145/D145,3)*-100,D145&gt;0,J145*D145/100),-J145)</f>
+        <v>4.8</v>
+      </c>
+      <c r="N145">
+        <f>SUM($M$2:M145)</f>
+        <v>-9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
       <c r="A146" s="2">
         <v>45355</v>
       </c>
@@ -12453,6 +14391,1505 @@
       </c>
       <c r="D146">
         <v>-285</v>
+      </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G146" s="3">
+        <f>SUM($F$3:F146)/COUNT($F$3:F146)</f>
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="H146" t="b">
+        <v>1</v>
+      </c>
+      <c r="I146">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <v>22</v>
+      </c>
+      <c r="L146" s="5">
+        <f>SUM($K$2:K146)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M146" cm="1">
+        <f t="array" ref="M146">IF(E146,_xlfn.IFS(D146="","",J146="","",D146&lt;0,ROUND(J146/D146,3)*-100,D146&gt;0,J146*D146/100),-J146)</f>
+        <v>7.7</v>
+      </c>
+      <c r="N146">
+        <f>SUM($M$2:M146)</f>
+        <v>-1.4999999999999991</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14">
+      <c r="A147" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B147" t="s">
+        <v>209</v>
+      </c>
+      <c r="C147" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="D147">
+        <v>-130</v>
+      </c>
+      <c r="E147" t="b">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G147" s="3">
+        <f>SUM($F$3:F147)/COUNT($F$3:F147)</f>
+        <v>0.66206896551724137</v>
+      </c>
+      <c r="H147" t="b">
+        <v>1</v>
+      </c>
+      <c r="I147">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J147">
+        <v>23</v>
+      </c>
+      <c r="L147" s="5">
+        <f>SUM($K$2:K147)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M147" cm="1">
+        <f t="array" ref="M147">IF(E147,_xlfn.IFS(D147="","",J147="","",D147&lt;0,ROUND(J147/D147,3)*-100,D147&gt;0,J147*D147/100),-J147)</f>
+        <v>17.7</v>
+      </c>
+      <c r="N147">
+        <f>SUM($M$2:M147)</f>
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="A148" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B148" t="s">
+        <v>58</v>
+      </c>
+      <c r="C148" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="D148">
+        <v>-162</v>
+      </c>
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G148" s="3">
+        <f>SUM($F$3:F148)/COUNT($F$3:F148)</f>
+        <v>0.66438356164383561</v>
+      </c>
+      <c r="H148" t="b">
+        <v>1</v>
+      </c>
+      <c r="I148">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>24</v>
+      </c>
+      <c r="L148" s="5">
+        <f>SUM($K$2:K148)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M148" cm="1">
+        <f t="array" ref="M148">IF(E148,_xlfn.IFS(D148="","",J148="","",D148&lt;0,ROUND(J148/D148,3)*-100,D148&gt;0,J148*D148/100),-J148)</f>
+        <v>14.799999999999999</v>
+      </c>
+      <c r="N148">
+        <f>SUM($M$2:M148)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B149" t="s">
+        <v>324</v>
+      </c>
+      <c r="C149" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="D149">
+        <v>105</v>
+      </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G149" s="3">
+        <f>SUM($F$3:F149)/COUNT($F$3:F149)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H149" t="b">
+        <v>1</v>
+      </c>
+      <c r="I149">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J149">
+        <v>25</v>
+      </c>
+      <c r="L149" s="5">
+        <f>SUM($K$2:K149)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M149" cm="1">
+        <f t="array" ref="M149">IF(E149,_xlfn.IFS(D149="","",J149="","",D149&lt;0,ROUND(J149/D149,3)*-100,D149&gt;0,J149*D149/100),-J149)</f>
+        <v>26.25</v>
+      </c>
+      <c r="N149">
+        <f>SUM($M$2:M149)</f>
+        <v>57.25</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B150" t="s">
+        <v>328</v>
+      </c>
+      <c r="C150" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D150">
+        <v>-230</v>
+      </c>
+      <c r="E150" t="b">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G150" s="3">
+        <f>SUM($F$3:F150)/COUNT($F$3:F150)</f>
+        <v>0.66216216216216217</v>
+      </c>
+      <c r="H150" t="b">
+        <v>1</v>
+      </c>
+      <c r="I150">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J150">
+        <v>26</v>
+      </c>
+      <c r="L150" s="5">
+        <f>SUM($K$2:K150)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M150" cm="1">
+        <f t="array" ref="M150">IF(E150,_xlfn.IFS(D150="","",J150="","",D150&lt;0,ROUND(J150/D150,3)*-100,D150&gt;0,J150*D150/100),-J150)</f>
+        <v>-26</v>
+      </c>
+      <c r="N150">
+        <f>SUM($M$2:M150)</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
+      <c r="A151" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B151" t="s">
+        <v>329</v>
+      </c>
+      <c r="C151" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D151">
+        <v>-4000</v>
+      </c>
+      <c r="E151" t="b">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G151" s="3">
+        <f>SUM($F$3:F151)/COUNT($F$3:F151)</f>
+        <v>0.65771812080536918</v>
+      </c>
+      <c r="H151" t="b">
+        <v>1</v>
+      </c>
+      <c r="I151">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J151">
+        <v>27</v>
+      </c>
+      <c r="L151" s="5">
+        <f>SUM($K$2:K151)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M151" cm="1">
+        <f t="array" ref="M151">IF(E151,_xlfn.IFS(D151="","",J151="","",D151&lt;0,ROUND(J151/D151,3)*-100,D151&gt;0,J151*D151/100),-J151)</f>
+        <v>-27</v>
+      </c>
+      <c r="N151">
+        <f>SUM($M$2:M151)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14">
+      <c r="B152" t="s">
+        <v>333</v>
+      </c>
+      <c r="C152" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D152">
+        <v>-245</v>
+      </c>
+      <c r="E152" t="b">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G152" s="3">
+        <f>SUM($F$3:F152)/COUNT($F$3:F152)</f>
+        <v>0.65333333333333332</v>
+      </c>
+      <c r="H152" t="b">
+        <v>1</v>
+      </c>
+      <c r="I152">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J152">
+        <v>28</v>
+      </c>
+      <c r="L152" s="5">
+        <f>SUM($K$2:K152)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M152" cm="1">
+        <f t="array" ref="M152">IF(E152,_xlfn.IFS(D152="","",J152="","",D152&lt;0,ROUND(J152/D152,3)*-100,D152&gt;0,J152*D152/100),-J152)</f>
+        <v>-28</v>
+      </c>
+      <c r="N152">
+        <f>SUM($M$2:M152)</f>
+        <v>-23.75</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="B153" t="s">
+        <v>334</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D153">
+        <v>-1650</v>
+      </c>
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G153" s="3">
+        <f>SUM($F$3:F153)/COUNT($F$3:F153)</f>
+        <v>0.6556291390728477</v>
+      </c>
+      <c r="H153" t="b">
+        <v>1</v>
+      </c>
+      <c r="I153">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J153">
+        <v>29</v>
+      </c>
+      <c r="L153" s="5">
+        <f>SUM($K$2:K153)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M153" cm="1">
+        <f t="array" ref="M153">IF(E153,_xlfn.IFS(D153="","",J153="","",D153&lt;0,ROUND(J153/D153,3)*-100,D153&gt;0,J153*D153/100),-J153)</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="N153">
+        <f>SUM($M$2:M153)</f>
+        <v>-21.95</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="B154" t="s">
+        <v>337</v>
+      </c>
+      <c r="C154" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="D154">
+        <v>114</v>
+      </c>
+      <c r="E154" t="b">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G154" s="3">
+        <f>SUM($F$3:F154)/COUNT($F$3:F154)</f>
+        <v>0.65131578947368418</v>
+      </c>
+      <c r="H154" t="b">
+        <v>1</v>
+      </c>
+      <c r="I154">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J154">
+        <v>30</v>
+      </c>
+      <c r="L154" s="5">
+        <f>SUM($K$2:K154)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M154" cm="1">
+        <f t="array" ref="M154">IF(E154,_xlfn.IFS(D154="","",J154="","",D154&lt;0,ROUND(J154/D154,3)*-100,D154&gt;0,J154*D154/100),-J154)</f>
+        <v>-30</v>
+      </c>
+      <c r="N154">
+        <f>SUM($M$2:M154)</f>
+        <v>-51.95</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14">
+      <c r="B155" t="s">
+        <v>338</v>
+      </c>
+      <c r="C155" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D155">
+        <v>114</v>
+      </c>
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G155" s="3">
+        <f>SUM($F$3:F155)/COUNT($F$3:F155)</f>
+        <v>0.65359477124183007</v>
+      </c>
+      <c r="H155" t="b">
+        <v>1</v>
+      </c>
+      <c r="I155">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J155">
+        <v>31</v>
+      </c>
+      <c r="L155" s="5">
+        <f>SUM($K$2:K155)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M155" cm="1">
+        <f t="array" ref="M155">IF(E155,_xlfn.IFS(D155="","",J155="","",D155&lt;0,ROUND(J155/D155,3)*-100,D155&gt;0,J155*D155/100),-J155)</f>
+        <v>35.340000000000003</v>
+      </c>
+      <c r="N155">
+        <f>SUM($M$2:M155)</f>
+        <v>-16.61</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="B156" t="s">
+        <v>343</v>
+      </c>
+      <c r="C156" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D156">
+        <v>-298</v>
+      </c>
+      <c r="E156" t="b">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G156" s="3">
+        <f>SUM($F$3:F156)/COUNT($F$3:F156)</f>
+        <v>0.64935064935064934</v>
+      </c>
+      <c r="H156" t="b">
+        <v>1</v>
+      </c>
+      <c r="I156">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J156">
+        <v>32</v>
+      </c>
+      <c r="L156" s="5">
+        <f>SUM($K$2:K156)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M156" cm="1">
+        <f t="array" ref="M156">IF(E156,_xlfn.IFS(D156="","",J156="","",D156&lt;0,ROUND(J156/D156,3)*-100,D156&gt;0,J156*D156/100),-J156)</f>
+        <v>-32</v>
+      </c>
+      <c r="N156">
+        <f>SUM($M$2:M156)</f>
+        <v>-48.61</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="B157" t="s">
+        <v>344</v>
+      </c>
+      <c r="C157" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="D157">
+        <v>270</v>
+      </c>
+      <c r="E157" t="b">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G157" s="3">
+        <f>SUM($F$3:F157)/COUNT($F$3:F157)</f>
+        <v>0.64516129032258063</v>
+      </c>
+      <c r="H157" t="b">
+        <v>1</v>
+      </c>
+      <c r="I157">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J157">
+        <v>33</v>
+      </c>
+      <c r="L157" s="5">
+        <f>SUM($K$2:K157)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M157" cm="1">
+        <f t="array" ref="M157">IF(E157,_xlfn.IFS(D157="","",J157="","",D157&lt;0,ROUND(J157/D157,3)*-100,D157&gt;0,J157*D157/100),-J157)</f>
+        <v>-33</v>
+      </c>
+      <c r="N157">
+        <f>SUM($M$2:M157)</f>
+        <v>-81.61</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14">
+      <c r="B158" t="s">
+        <v>347</v>
+      </c>
+      <c r="C158" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="D158">
+        <v>-395</v>
+      </c>
+      <c r="E158" t="b">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G158" s="3">
+        <f>SUM($F$3:F158)/COUNT($F$3:F158)</f>
+        <v>0.64743589743589747</v>
+      </c>
+      <c r="H158" t="b">
+        <v>1</v>
+      </c>
+      <c r="I158">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J158">
+        <v>34</v>
+      </c>
+      <c r="L158" s="5">
+        <f>SUM($K$2:K158)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M158" cm="1">
+        <f t="array" ref="M158">IF(E158,_xlfn.IFS(D158="","",J158="","",D158&lt;0,ROUND(J158/D158,3)*-100,D158&gt;0,J158*D158/100),-J158)</f>
+        <v>8.6</v>
+      </c>
+      <c r="N158">
+        <f>SUM($M$2:M158)</f>
+        <v>-73.010000000000005</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14">
+      <c r="B159" t="s">
+        <v>348</v>
+      </c>
+      <c r="C159" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="D159">
+        <v>-425</v>
+      </c>
+      <c r="E159" t="b">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G159" s="3">
+        <f>SUM($F$3:F159)/COUNT($F$3:F159)</f>
+        <v>0.64331210191082799</v>
+      </c>
+      <c r="H159" t="b">
+        <v>1</v>
+      </c>
+      <c r="I159">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J159">
+        <v>35</v>
+      </c>
+      <c r="L159" s="5">
+        <f>SUM($K$2:K159)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M159" cm="1">
+        <f t="array" ref="M159">IF(E159,_xlfn.IFS(D159="","",J159="","",D159&lt;0,ROUND(J159/D159,3)*-100,D159&gt;0,J159*D159/100),-J159)</f>
+        <v>-35</v>
+      </c>
+      <c r="N159">
+        <f>SUM($M$2:M159)</f>
+        <v>-108.01</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="B160" t="s">
+        <v>352</v>
+      </c>
+      <c r="C160" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D160">
+        <v>180</v>
+      </c>
+      <c r="E160" t="b">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G160" s="3">
+        <f>SUM($F$3:F160)/COUNT($F$3:F160)</f>
+        <v>0.63924050632911389</v>
+      </c>
+      <c r="H160" t="b">
+        <v>1</v>
+      </c>
+      <c r="I160">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J160">
+        <v>36</v>
+      </c>
+      <c r="L160" s="5">
+        <f>SUM($K$2:K160)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M160" cm="1">
+        <f t="array" ref="M160">IF(E160,_xlfn.IFS(D160="","",J160="","",D160&lt;0,ROUND(J160/D160,3)*-100,D160&gt;0,J160*D160/100),-J160)</f>
+        <v>-36</v>
+      </c>
+      <c r="N160">
+        <f>SUM($M$2:M160)</f>
+        <v>-144.01</v>
+      </c>
+    </row>
+    <row r="161" spans="2:14">
+      <c r="B161" t="s">
+        <v>239</v>
+      </c>
+      <c r="C161" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="D161">
+        <v>120</v>
+      </c>
+      <c r="E161" t="b">
+        <v>1</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G161" s="3">
+        <f>SUM($F$3:F161)/COUNT($F$3:F161)</f>
+        <v>0.64150943396226412</v>
+      </c>
+      <c r="H161" t="b">
+        <v>1</v>
+      </c>
+      <c r="I161">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J161">
+        <v>37</v>
+      </c>
+      <c r="L161" s="5">
+        <f>SUM($K$2:K161)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M161" cm="1">
+        <f t="array" ref="M161">IF(E161,_xlfn.IFS(D161="","",J161="","",D161&lt;0,ROUND(J161/D161,3)*-100,D161&gt;0,J161*D161/100),-J161)</f>
+        <v>44.4</v>
+      </c>
+      <c r="N161">
+        <f>SUM($M$2:M161)</f>
+        <v>-99.609999999999985</v>
+      </c>
+    </row>
+    <row r="162" spans="2:14">
+      <c r="B162" t="s">
+        <v>357</v>
+      </c>
+      <c r="C162" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="D162">
+        <v>-1800</v>
+      </c>
+      <c r="E162" t="b">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G162" s="3">
+        <f>SUM($F$3:F162)/COUNT($F$3:F162)</f>
+        <v>0.64375000000000004</v>
+      </c>
+      <c r="H162" t="b">
+        <v>1</v>
+      </c>
+      <c r="I162">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J162">
+        <v>38</v>
+      </c>
+      <c r="L162" s="5">
+        <f>SUM($K$2:K162)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M162" cm="1">
+        <f t="array" ref="M162">IF(E162,_xlfn.IFS(D162="","",J162="","",D162&lt;0,ROUND(J162/D162,3)*-100,D162&gt;0,J162*D162/100),-J162)</f>
+        <v>2.1</v>
+      </c>
+      <c r="N162">
+        <f>SUM($M$2:M162)</f>
+        <v>-97.509999999999991</v>
+      </c>
+    </row>
+    <row r="163" spans="2:14">
+      <c r="B163" t="s">
+        <v>358</v>
+      </c>
+      <c r="C163" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D163">
+        <v>-355</v>
+      </c>
+      <c r="E163" t="b">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G163" s="3">
+        <f>SUM($F$3:F163)/COUNT($F$3:F163)</f>
+        <v>0.64596273291925466</v>
+      </c>
+      <c r="H163" t="b">
+        <v>1</v>
+      </c>
+      <c r="I163">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J163">
+        <v>39</v>
+      </c>
+      <c r="L163" s="5">
+        <f>SUM($K$2:K163)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M163" cm="1">
+        <f t="array" ref="M163">IF(E163,_xlfn.IFS(D163="","",J163="","",D163&lt;0,ROUND(J163/D163,3)*-100,D163&gt;0,J163*D163/100),-J163)</f>
+        <v>11</v>
+      </c>
+      <c r="N163">
+        <f>SUM($M$2:M163)</f>
+        <v>-86.509999999999991</v>
+      </c>
+    </row>
+    <row r="164" spans="2:14">
+      <c r="B164" t="s">
+        <v>359</v>
+      </c>
+      <c r="C164" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D164">
+        <v>-395</v>
+      </c>
+      <c r="E164" t="b">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G164" s="3">
+        <f>SUM($F$3:F164)/COUNT($F$3:F164)</f>
+        <v>0.64814814814814814</v>
+      </c>
+      <c r="H164" t="b">
+        <v>1</v>
+      </c>
+      <c r="I164">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J164">
+        <v>40</v>
+      </c>
+      <c r="L164" s="5">
+        <f>SUM($K$2:K164)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M164" cm="1">
+        <f t="array" ref="M164">IF(E164,_xlfn.IFS(D164="","",J164="","",D164&lt;0,ROUND(J164/D164,3)*-100,D164&gt;0,J164*D164/100),-J164)</f>
+        <v>10.100000000000001</v>
+      </c>
+      <c r="N164">
+        <f>SUM($M$2:M164)</f>
+        <v>-76.41</v>
+      </c>
+    </row>
+    <row r="165" spans="2:14">
+      <c r="B165" t="s">
+        <v>360</v>
+      </c>
+      <c r="C165" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="D165">
+        <v>-675</v>
+      </c>
+      <c r="E165" t="b">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G165" s="3">
+        <f>SUM($F$3:F165)/COUNT($F$3:F165)</f>
+        <v>0.65030674846625769</v>
+      </c>
+      <c r="H165" t="b">
+        <v>1</v>
+      </c>
+      <c r="I165">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J165">
+        <v>41</v>
+      </c>
+      <c r="L165" s="5">
+        <f>SUM($K$2:K165)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M165" cm="1">
+        <f t="array" ref="M165">IF(E165,_xlfn.IFS(D165="","",J165="","",D165&lt;0,ROUND(J165/D165,3)*-100,D165&gt;0,J165*D165/100),-J165)</f>
+        <v>6.1</v>
+      </c>
+      <c r="N165">
+        <f>SUM($M$2:M165)</f>
+        <v>-70.31</v>
+      </c>
+    </row>
+    <row r="166" spans="2:14">
+      <c r="B166" t="s">
+        <v>364</v>
+      </c>
+      <c r="C166" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="D166">
+        <v>-230</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G166" s="3">
+        <f>SUM($F$3:F166)/COUNT($F$3:F166)</f>
+        <v>0.64634146341463417</v>
+      </c>
+      <c r="H166" t="b">
+        <v>1</v>
+      </c>
+      <c r="I166">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J166">
+        <v>42</v>
+      </c>
+      <c r="L166" s="5">
+        <f>SUM($K$2:K166)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M166" cm="1">
+        <f t="array" ref="M166">IF(E166,_xlfn.IFS(D166="","",J166="","",D166&lt;0,ROUND(J166/D166,3)*-100,D166&gt;0,J166*D166/100),-J166)</f>
+        <v>-42</v>
+      </c>
+      <c r="N166">
+        <f>SUM($M$2:M166)</f>
+        <v>-112.31</v>
+      </c>
+    </row>
+    <row r="167" spans="2:14">
+      <c r="B167" t="s">
+        <v>191</v>
+      </c>
+      <c r="C167" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="D167">
+        <v>-148</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G167" s="3">
+        <f>SUM($F$3:F167)/COUNT($F$3:F167)</f>
+        <v>0.64242424242424245</v>
+      </c>
+      <c r="H167" t="b">
+        <v>1</v>
+      </c>
+      <c r="I167">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J167">
+        <v>43</v>
+      </c>
+      <c r="L167" s="5">
+        <f>SUM($K$2:K167)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M167" cm="1">
+        <f t="array" ref="M167">IF(E167,_xlfn.IFS(D167="","",J167="","",D167&lt;0,ROUND(J167/D167,3)*-100,D167&gt;0,J167*D167/100),-J167)</f>
+        <v>-43</v>
+      </c>
+      <c r="N167">
+        <f>SUM($M$2:M167)</f>
+        <v>-155.31</v>
+      </c>
+    </row>
+    <row r="168" spans="2:14">
+      <c r="B168" t="s">
+        <v>367</v>
+      </c>
+      <c r="C168" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="D168">
+        <v>-850</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G168" s="3">
+        <f>SUM($F$3:F168)/COUNT($F$3:F168)</f>
+        <v>0.63855421686746983</v>
+      </c>
+      <c r="H168" t="b">
+        <v>1</v>
+      </c>
+      <c r="I168">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J168">
+        <v>44</v>
+      </c>
+      <c r="L168" s="5">
+        <f>SUM($K$2:K168)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M168" cm="1">
+        <f t="array" ref="M168">IF(E168,_xlfn.IFS(D168="","",J168="","",D168&lt;0,ROUND(J168/D168,3)*-100,D168&gt;0,J168*D168/100),-J168)</f>
+        <v>-44</v>
+      </c>
+      <c r="N168">
+        <f>SUM($M$2:M168)</f>
+        <v>-199.31</v>
+      </c>
+    </row>
+    <row r="169" spans="2:14">
+      <c r="B169" t="s">
+        <v>46</v>
+      </c>
+      <c r="C169" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D169">
+        <v>-310</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G169" s="3">
+        <f>SUM($F$3:F169)/COUNT($F$3:F169)</f>
+        <v>0.6347305389221557</v>
+      </c>
+      <c r="H169" t="b">
+        <v>1</v>
+      </c>
+      <c r="I169">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J169">
+        <v>45</v>
+      </c>
+      <c r="L169" s="5">
+        <f>SUM($K$2:K169)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M169" cm="1">
+        <f t="array" ref="M169">IF(E169,_xlfn.IFS(D169="","",J169="","",D169&lt;0,ROUND(J169/D169,3)*-100,D169&gt;0,J169*D169/100),-J169)</f>
+        <v>-45</v>
+      </c>
+      <c r="N169">
+        <f>SUM($M$2:M169)</f>
+        <v>-244.31</v>
+      </c>
+    </row>
+    <row r="170" spans="2:14">
+      <c r="B170" t="s">
+        <v>368</v>
+      </c>
+      <c r="C170" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D170">
+        <v>-162</v>
+      </c>
+      <c r="F170">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G170" s="3">
+        <f>SUM($F$3:F170)/COUNT($F$3:F170)</f>
+        <v>0.63095238095238093</v>
+      </c>
+      <c r="H170" t="b">
+        <v>1</v>
+      </c>
+      <c r="I170">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <v>46</v>
+      </c>
+      <c r="L170" s="5">
+        <f>SUM($K$2:K170)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M170" cm="1">
+        <f t="array" ref="M170">IF(E170,_xlfn.IFS(D170="","",J170="","",D170&lt;0,ROUND(J170/D170,3)*-100,D170&gt;0,J170*D170/100),-J170)</f>
+        <v>-46</v>
+      </c>
+      <c r="N170">
+        <f>SUM($M$2:M170)</f>
+        <v>-290.31</v>
+      </c>
+    </row>
+    <row r="171" spans="2:14">
+      <c r="B171" t="s">
+        <v>372</v>
+      </c>
+      <c r="C171" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D171">
+        <v>154</v>
+      </c>
+      <c r="F171">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G171" s="3">
+        <f>SUM($F$3:F171)/COUNT($F$3:F171)</f>
+        <v>0.62721893491124259</v>
+      </c>
+      <c r="H171" t="b">
+        <v>1</v>
+      </c>
+      <c r="I171">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J171">
+        <v>47</v>
+      </c>
+      <c r="L171" s="5">
+        <f>SUM($K$2:K171)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M171" cm="1">
+        <f t="array" ref="M171">IF(E171,_xlfn.IFS(D171="","",J171="","",D171&lt;0,ROUND(J171/D171,3)*-100,D171&gt;0,J171*D171/100),-J171)</f>
+        <v>-47</v>
+      </c>
+      <c r="N171">
+        <f>SUM($M$2:M171)</f>
+        <v>-337.31</v>
+      </c>
+    </row>
+    <row r="172" spans="2:14">
+      <c r="B172" t="s">
+        <v>373</v>
+      </c>
+      <c r="C172" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D172">
+        <v>150</v>
+      </c>
+      <c r="F172">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G172" s="3">
+        <f>SUM($F$3:F172)/COUNT($F$3:F172)</f>
+        <v>0.62352941176470589</v>
+      </c>
+      <c r="H172" t="b">
+        <v>1</v>
+      </c>
+      <c r="I172">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J172">
+        <v>48</v>
+      </c>
+      <c r="L172" s="5">
+        <f>SUM($K$2:K172)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M172" cm="1">
+        <f t="array" ref="M172">IF(E172,_xlfn.IFS(D172="","",J172="","",D172&lt;0,ROUND(J172/D172,3)*-100,D172&gt;0,J172*D172/100),-J172)</f>
+        <v>-48</v>
+      </c>
+      <c r="N172">
+        <f>SUM($M$2:M172)</f>
+        <v>-385.31</v>
+      </c>
+    </row>
+    <row r="173" spans="2:14">
+      <c r="B173" t="s">
+        <v>378</v>
+      </c>
+      <c r="C173" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="D173">
+        <v>-298</v>
+      </c>
+      <c r="F173">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G173" s="3">
+        <f>SUM($F$3:F173)/COUNT($F$3:F173)</f>
+        <v>0.61988304093567248</v>
+      </c>
+      <c r="H173" t="b">
+        <v>1</v>
+      </c>
+      <c r="I173">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J173">
+        <v>49</v>
+      </c>
+      <c r="L173" s="5">
+        <f>SUM($K$2:K173)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M173" cm="1">
+        <f t="array" ref="M173">IF(E173,_xlfn.IFS(D173="","",J173="","",D173&lt;0,ROUND(J173/D173,3)*-100,D173&gt;0,J173*D173/100),-J173)</f>
+        <v>-49</v>
+      </c>
+      <c r="N173">
+        <f>SUM($M$2:M173)</f>
+        <v>-434.31</v>
+      </c>
+    </row>
+    <row r="174" spans="2:14">
+      <c r="B174" t="s">
+        <v>379</v>
+      </c>
+      <c r="C174" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D174">
+        <v>-850</v>
+      </c>
+      <c r="F174">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G174" s="3">
+        <f>SUM($F$3:F174)/COUNT($F$3:F174)</f>
+        <v>0.61627906976744184</v>
+      </c>
+      <c r="H174" t="b">
+        <v>1</v>
+      </c>
+      <c r="I174">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J174">
+        <v>50</v>
+      </c>
+      <c r="L174" s="5">
+        <f>SUM($K$2:K174)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M174" cm="1">
+        <f t="array" ref="M174">IF(E174,_xlfn.IFS(D174="","",J174="","",D174&lt;0,ROUND(J174/D174,3)*-100,D174&gt;0,J174*D174/100),-J174)</f>
+        <v>-50</v>
+      </c>
+      <c r="N174">
+        <f>SUM($M$2:M174)</f>
+        <v>-484.31</v>
+      </c>
+    </row>
+    <row r="175" spans="2:14">
+      <c r="B175" t="s">
+        <v>382</v>
+      </c>
+      <c r="C175" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D175">
+        <v>-800</v>
+      </c>
+      <c r="F175">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G175" s="3">
+        <f>SUM($F$3:F175)/COUNT($F$3:F175)</f>
+        <v>0.61271676300578037</v>
+      </c>
+      <c r="H175" t="b">
+        <v>1</v>
+      </c>
+      <c r="I175">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J175">
+        <v>51</v>
+      </c>
+      <c r="L175" s="5">
+        <f>SUM($K$2:K175)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M175" cm="1">
+        <f t="array" ref="M175">IF(E175,_xlfn.IFS(D175="","",J175="","",D175&lt;0,ROUND(J175/D175,3)*-100,D175&gt;0,J175*D175/100),-J175)</f>
+        <v>-51</v>
+      </c>
+      <c r="N175">
+        <f>SUM($M$2:M175)</f>
+        <v>-535.30999999999995</v>
+      </c>
+    </row>
+    <row r="176" spans="2:14">
+      <c r="B176" t="s">
+        <v>383</v>
+      </c>
+      <c r="C176" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="D176">
+        <v>-470</v>
+      </c>
+      <c r="F176">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G176" s="3">
+        <f>SUM($F$3:F176)/COUNT($F$3:F176)</f>
+        <v>0.60919540229885061</v>
+      </c>
+      <c r="H176" t="b">
+        <v>1</v>
+      </c>
+      <c r="I176">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J176">
+        <v>52</v>
+      </c>
+      <c r="L176" s="5">
+        <f>SUM($K$2:K176)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M176" cm="1">
+        <f t="array" ref="M176">IF(E176,_xlfn.IFS(D176="","",J176="","",D176&lt;0,ROUND(J176/D176,3)*-100,D176&gt;0,J176*D176/100),-J176)</f>
+        <v>-52</v>
+      </c>
+      <c r="N176">
+        <f>SUM($M$2:M176)</f>
+        <v>-587.30999999999995</v>
+      </c>
+    </row>
+    <row r="177" spans="2:14">
+      <c r="B177" t="s">
+        <v>187</v>
+      </c>
+      <c r="C177" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D177">
+        <v>-1100</v>
+      </c>
+      <c r="F177">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G177" s="3">
+        <f>SUM($F$3:F177)/COUNT($F$3:F177)</f>
+        <v>0.60571428571428576</v>
+      </c>
+      <c r="H177" t="b">
+        <v>1</v>
+      </c>
+      <c r="I177">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J177">
+        <v>53</v>
+      </c>
+      <c r="L177" s="5">
+        <f>SUM($K$2:K177)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M177" cm="1">
+        <f t="array" ref="M177">IF(E177,_xlfn.IFS(D177="","",J177="","",D177&lt;0,ROUND(J177/D177,3)*-100,D177&gt;0,J177*D177/100),-J177)</f>
+        <v>-53</v>
+      </c>
+      <c r="N177">
+        <f>SUM($M$2:M177)</f>
+        <v>-640.30999999999995</v>
+      </c>
+    </row>
+    <row r="178" spans="2:14">
+      <c r="B178" t="s">
+        <v>385</v>
+      </c>
+      <c r="C178" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="D178">
+        <v>-345</v>
+      </c>
+      <c r="F178">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G178" s="3">
+        <f>SUM($F$3:F178)/COUNT($F$3:F178)</f>
+        <v>0.60227272727272729</v>
+      </c>
+      <c r="H178" t="b">
+        <v>1</v>
+      </c>
+      <c r="I178">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J178">
+        <v>54</v>
+      </c>
+      <c r="L178" s="5">
+        <f>SUM($K$2:K178)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M178" cm="1">
+        <f t="array" ref="M178">IF(E178,_xlfn.IFS(D178="","",J178="","",D178&lt;0,ROUND(J178/D178,3)*-100,D178&gt;0,J178*D178/100),-J178)</f>
+        <v>-54</v>
+      </c>
+      <c r="N178">
+        <f>SUM($M$2:M178)</f>
+        <v>-694.31</v>
+      </c>
+    </row>
+    <row r="179" spans="2:14">
+      <c r="B179" t="s">
+        <v>234</v>
+      </c>
+      <c r="C179" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D179">
+        <v>-250</v>
+      </c>
+      <c r="F179">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G179" s="3">
+        <f>SUM($F$3:F179)/COUNT($F$3:F179)</f>
+        <v>0.59887005649717517</v>
+      </c>
+      <c r="H179" t="b">
+        <v>1</v>
+      </c>
+      <c r="I179">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J179">
+        <v>55</v>
+      </c>
+      <c r="L179" s="5">
+        <f>SUM($K$2:K179)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M179" cm="1">
+        <f t="array" ref="M179">IF(E179,_xlfn.IFS(D179="","",J179="","",D179&lt;0,ROUND(J179/D179,3)*-100,D179&gt;0,J179*D179/100),-J179)</f>
+        <v>-55</v>
+      </c>
+      <c r="N179">
+        <f>SUM($M$2:M179)</f>
+        <v>-749.31</v>
+      </c>
+    </row>
+    <row r="180" spans="2:14">
+      <c r="B180" t="s">
+        <v>389</v>
+      </c>
+      <c r="C180" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="D180">
+        <v>-148</v>
+      </c>
+      <c r="F180">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G180" s="3">
+        <f>SUM($F$3:F180)/COUNT($F$3:F180)</f>
+        <v>0.5955056179775281</v>
+      </c>
+      <c r="H180" t="b">
+        <v>1</v>
+      </c>
+      <c r="I180">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J180">
+        <v>56</v>
+      </c>
+      <c r="L180" s="5">
+        <f>SUM($K$2:K180)</f>
+        <v>-2.3800000000000003</v>
+      </c>
+      <c r="M180" cm="1">
+        <f t="array" ref="M180">IF(E180,_xlfn.IFS(D180="","",J180="","",D180&lt;0,ROUND(J180/D180,3)*-100,D180&gt;0,J180*D180/100),-J180)</f>
+        <v>-56</v>
+      </c>
+      <c r="N180">
+        <f>SUM($M$2:M180)</f>
+        <v>-805.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>